<commit_message>
data update for 8/22
</commit_message>
<xml_diff>
--- a/next_week.xlsx
+++ b/next_week.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rboehm/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC29AB7D-BB4D-6942-A4CD-033FB4BD0189}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F09AB08F-C908-844F-8080-324EE9887DF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3560" windowWidth="35020" windowHeight="19680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SG Data" sheetId="1" r:id="rId1"/>
@@ -226,9 +226,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,12 +294,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -379,7 +384,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -397,6 +402,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -406,8 +414,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 1" xfId="2" builtinId="16"/>
@@ -745,160 +754,160 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="0">
-                  <c:v>7.182131594674444</c:v>
+                  <c:v>1.952226714230219</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0699334977116646</c:v>
+                  <c:v>0.92173287444541352</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.89704396159677</c:v>
+                  <c:v>1.6109009222038171</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.4496423548841779</c:v>
+                  <c:v>4.0428409707538684</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.6220640735251246</c:v>
+                  <c:v>-0.3656504095981995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.8024638302302822</c:v>
+                  <c:v>1.066680421632493</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.2351251047527834</c:v>
+                  <c:v>2.7416031909845779</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.3082320607377189</c:v>
+                  <c:v>4.8722050297272528</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.5925392102399343</c:v>
+                  <c:v>1.824526569249975</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.2</c:v>
+                  <c:v>1.6867000000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.678654475615569</c:v>
+                  <c:v>3.6976566810100429</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.6333841407503211</c:v>
+                  <c:v>0.85765789170047335</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-2.4</c:v>
+                  <c:v>-3.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.5897739721587323</c:v>
+                  <c:v>0.90397531552482302</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.7061469513150129</c:v>
+                  <c:v>1.084444709735864</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.0011892011473549</c:v>
+                  <c:v>1.3155841759421401</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.1421627409326023</c:v>
+                  <c:v>-3.3857023090733802E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.0556767927575361</c:v>
+                  <c:v>1.1339414525998219</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.6927302393753321</c:v>
+                  <c:v>2.9471173091810901</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.2057078568512329</c:v>
+                  <c:v>1.698513515310103</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9.606641929499073</c:v>
+                  <c:v>3.5139095255744999</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.5012369658556528</c:v>
+                  <c:v>1.7200992758057929</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9.6141355754072517</c:v>
+                  <c:v>4.5705902515723276</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7.6909690090531244</c:v>
+                  <c:v>2.853976959114358</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>8.0977583580367547</c:v>
+                  <c:v>-0.35076249485863709</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4.2454046893045598</c:v>
+                  <c:v>-0.6715656589898179</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>5.0925920537711651</c:v>
+                  <c:v>3.6997261891173798E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>8.1</c:v>
+                  <c:v>-9.1</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.8211160073263648</c:v>
+                  <c:v>2.3594707781631499</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>6.8730564758989017</c:v>
+                  <c:v>3.656372797142176</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>9.9847512911117153</c:v>
+                  <c:v>3.901217438396968</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>7.1051307974837261</c:v>
+                  <c:v>1.7557482065236309</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>8.3164511095824363</c:v>
+                  <c:v>1.345882270796938</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>6.6621963030695772</c:v>
+                  <c:v>4.6367042716560203</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>9.543301673887477</c:v>
+                  <c:v>-2.512053672974583</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3.8390158737684938</c:v>
+                  <c:v>-0.41384953209198372</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>5.5037833564203051</c:v>
+                  <c:v>3.4079576584502052</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>8.5871894165134908</c:v>
+                  <c:v>1.983040472960746</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>8.9987135236899913</c:v>
+                  <c:v>4.0209003783698556</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>8.2138451223600395</c:v>
+                  <c:v>3.2707898537226758</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.1599999999999999</c:v>
+                  <c:v>8.7900000000000009</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>9.0014269498946007</c:v>
+                  <c:v>1.422161443832956</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4.2694705403268776</c:v>
+                  <c:v>8.9057695083403055E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>6.1606707707202073</c:v>
+                  <c:v>1.479616139570489</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>5.8971505894804439</c:v>
+                  <c:v>4.5097040090413792E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>7.8</c:v>
+                  <c:v>3.726799999999999</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>11.54993564993565</c:v>
+                  <c:v>3.5231043114543108</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>7.9608780975835014</c:v>
+                  <c:v>2.5975384144006131</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>10.78425196850394</c:v>
+                  <c:v>3.668004172811659</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>8.0610765950567753</c:v>
+                  <c:v>-0.37215907946615512</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>5.2004958925773748</c:v>
+                  <c:v>-0.66961514013486523</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>11.3</c:v>
+                  <c:v>-5.8999999999999986</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1401,160 +1410,160 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="0">
-                  <c:v>0.92876007738819211</c:v>
+                  <c:v>1.8816809396815011</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.011871207653904</c:v>
+                  <c:v>-0.13684794955315249</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.7891723060905722</c:v>
+                  <c:v>1.5944195316392571</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.02115301407443</c:v>
+                  <c:v>1.8687629395474969</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.857241882840581</c:v>
+                  <c:v>-0.21154512843720161</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.7554689761360209</c:v>
+                  <c:v>4.9412887297431736</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.36619178738177888</c:v>
+                  <c:v>0.97588659549228962</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-5.7728829523413498</c:v>
+                  <c:v>2.2058329381210382</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.30168700048458902</c:v>
+                  <c:v>-0.71507897940681897</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-1.8</c:v>
+                  <c:v>-0.85229999999999995</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.10344826604216061</c:v>
+                  <c:v>3.1007717736790998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.87001695881590357</c:v>
+                  <c:v>1.2442931006904361</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-1.4</c:v>
+                  <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.445243494719439</c:v>
+                  <c:v>-0.51896038999611593</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9.4609577248970123E-2</c:v>
+                  <c:v>2.059336055689327</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.35862798818494018</c:v>
+                  <c:v>1.3836458010305659</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.125743693918053</c:v>
+                  <c:v>3.278806632706547</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.18545035632577819</c:v>
+                  <c:v>-0.44546958509614681</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.9921223457459658</c:v>
+                  <c:v>-0.57083325002379515</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-0.70125557741213973</c:v>
+                  <c:v>-0.62481056998156903</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.6493506493506498</c:v>
+                  <c:v>2.3920596738324691</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>9.561439378450215E-2</c:v>
+                  <c:v>-0.35240948592411259</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.31823436678928008</c:v>
+                  <c:v>1.976588836477988</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-0.46805123518739628</c:v>
+                  <c:v>0.90560901382307935</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.34735147219181878</c:v>
+                  <c:v>-0.2130501858234348</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.407137606983017</c:v>
+                  <c:v>-2.6188696749271898</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.128222826480554</c:v>
+                  <c:v>0.18811453368439379</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>5.2</c:v>
+                  <c:v>-12.4</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.55734966971934485</c:v>
+                  <c:v>5.517907403754454</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4.7747896778307144</c:v>
+                  <c:v>2.3116607333001529</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.84240282685512369</c:v>
+                  <c:v>1.4834379637151369</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-1.9344101441374619</c:v>
+                  <c:v>-0.27577313300434431</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.210525191929757</c:v>
+                  <c:v>2.9888207865388789</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1.423310368769088</c:v>
+                  <c:v>1.882629026883506</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>5.1958867938428996</c:v>
+                  <c:v>1.865211027121678</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1.917205337632232</c:v>
+                  <c:v>-0.51352497947364284</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3.5845977602382462</c:v>
+                  <c:v>-0.3830916636220083</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.50105294508293641</c:v>
+                  <c:v>0.60589875885424127</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.76167241920301221</c:v>
+                  <c:v>0.79869746176887924</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.1015085484411667</c:v>
+                  <c:v>1.232272042951843</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>7.3999999999999986</c:v>
+                  <c:v>0.36</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>4.065380249716231</c:v>
+                  <c:v>-0.79210946908384594</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2.3851167698482878</c:v>
+                  <c:v>-1.2343481117721229</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.60793745030012702</c:v>
+                  <c:v>0.96912108811170061</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>-1.471860660589787</c:v>
+                  <c:v>5.7562279821459574</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.6</c:v>
+                  <c:v>1.0561</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.3248391248391248</c:v>
+                  <c:v>2.1414968468468469</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.36874326612282599</c:v>
+                  <c:v>0.1197955112983531</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>-0.7338582677165354</c:v>
+                  <c:v>0.48709237442526238</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.62440781963251146</c:v>
+                  <c:v>0.92597965918349467</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>6.0345050626290311</c:v>
+                  <c:v>0.38545703390716612</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>3.6</c:v>
+                  <c:v>-9.8000000000000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2062,160 +2071,160 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="0">
-                  <c:v>1.543912039881753</c:v>
+                  <c:v>1.4858257782428781</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.649550173010381</c:v>
+                  <c:v>0.79489501496721382</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5714285714285714</c:v>
+                  <c:v>0.28564009348221242</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.93095660003266567</c:v>
+                  <c:v>2.6258305484334659</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.74903126015323229</c:v>
+                  <c:v>0.66645866145839117</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.3124914075953473</c:v>
+                  <c:v>5.4751741780354184</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.6519214653417928</c:v>
+                  <c:v>2.7850118794684779</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.194897111385903</c:v>
+                  <c:v>0.90535661506212473</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.81281448661144307</c:v>
+                  <c:v>1.0455667291188151</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.3</c:v>
+                  <c:v>0.70726915520599998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.05778935659065</c:v>
+                  <c:v>1.006799081740112</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.231103335617947</c:v>
+                  <c:v>1.4543830932502031</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.5999999999999996</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.1445691534194041</c:v>
+                  <c:v>0.19148508246355911</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.66341669515695256</c:v>
+                  <c:v>0.70817426939542294</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.48114958519685341</c:v>
+                  <c:v>0.47408561105547931</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.871280945030031E-2</c:v>
+                  <c:v>4.3761777562127832E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.29804323719423093</c:v>
+                  <c:v>0.16688931933052881</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.101350177127197</c:v>
+                  <c:v>1.006190380895204</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.97615678214525847</c:v>
+                  <c:v>0.63260642698065905</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.32148423005565863</c:v>
+                  <c:v>0.30041564370931401</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.005172766305459</c:v>
+                  <c:v>0.7125504121618339</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.96831318970047298</c:v>
+                  <c:v>0.69948790181621534</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.32568533194751198</c:v>
+                  <c:v>0.17101876605010141</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.6067087236882186</c:v>
+                  <c:v>0.44598518800130649</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.62082116043099922</c:v>
+                  <c:v>0.28818617965387272</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.081573410826616</c:v>
+                  <c:v>0.86012890175247969</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.3</c:v>
+                  <c:v>0.89999999999999991</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>5.9903186768858412E-2</c:v>
+                  <c:v>0.58834338560514676</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.0604764411687291</c:v>
+                  <c:v>1.015059119496855</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.47575428105463441</c:v>
+                  <c:v>0.38086996142046031</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.379577012043796</c:v>
+                  <c:v>1.0576684818707771</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.953987840829263</c:v>
+                  <c:v>2.4032291953466012</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1.220446568705549</c:v>
+                  <c:v>1.0208197090178961</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.46118949031643</c:v>
+                  <c:v>1.264622817443823</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.7790083848971241E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.002256900715857</c:v>
+                  <c:v>0.69851521178124309</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.24594845388298159</c:v>
+                  <c:v>0.28329072350077578</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.0805145905240039</c:v>
+                  <c:v>1.0121698219366579</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.52769024472008041</c:v>
+                  <c:v>0.49374888914639692</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.14000000000000001</c:v>
+                  <c:v>0.24</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.89164910004864617</c:v>
+                  <c:v>0.56467777387997586</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.39931592748831379</c:v>
+                  <c:v>0.1867615515124342</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1.250207301041562</c:v>
+                  <c:v>0.82328893356332067</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.585089773536539</c:v>
+                  <c:v>1.8979374906461579</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1.3</c:v>
+                  <c:v>1.078605200945</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.31872586872586872</c:v>
+                  <c:v>0.15414392726346529</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.55045405571802364</c:v>
+                  <c:v>0.54243718450119027</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.5228346456692909</c:v>
+                  <c:v>1.225596379651539</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1.296952993028597</c:v>
+                  <c:v>0.99747928025338373</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1.940579917154692</c:v>
+                  <c:v>1.261274230330673</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.8</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2721,43 +2730,43 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="0">
-                  <c:v>9.4010750793182093E-2</c:v>
+                  <c:v>5.4600258989583497E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.06</c:v>
+                  <c:v>8.1090260514783491E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.15228198194286799</c:v>
+                  <c:v>0.17696810873265381</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.36153471977310442</c:v>
+                  <c:v>0.29236685578686311</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.16139807582056881</c:v>
+                  <c:v>6.9247236220964944E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>6.6388784738578878E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.12745219366051511</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.1443366508712392</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8.7262569832402243E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.12982039669762999</c:v>
+                  <c:v>7.6015847167901718E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.7870030189393812E-2</c:v>
+                  <c:v>3.8643254915559839E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.70000000000000007</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -2766,40 +2775,40 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.944228419064549E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.435640472515015E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.0321485907049529E-2</c:v>
+                  <c:v>2.0176951867881321E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.10746607847069049</c:v>
+                  <c:v>1.033953705556667E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.1179159279508601</c:v>
+                  <c:v>0.12584750838499581</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>2.614863897822348E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>8.943772990015765E-2</c:v>
+                  <c:v>9.7076181428672956E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>6.7894386509873533E-2</c:v>
+                  <c:v>2.5955913351755601E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>6.9362802051866346E-2</c:v>
+                  <c:v>3.9200877355929697E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.0383515065444039E-2</c:v>
+                  <c:v>1.5154049855972679E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>0</c:v>
@@ -2808,37 +2817,37 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>8.2508554882863905E-2</c:v>
+                  <c:v>7.0631446540880508E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0</c:v>
+                  <c:v>4.8620957370760901E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>6.7337395826970597E-2</c:v>
+                  <c:v>5.1068703612935633E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.36968430762975069</c:v>
+                  <c:v>0.22871941013318581</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>8.6521506075509638E-2</c:v>
+                  <c:v>3.9378977358205468E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>9.4911222003017298E-2</c:v>
+                  <c:v>3.3983952833643782E-3</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.1026196398837813</c:v>
+                  <c:v>2.136345778536302E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1.4684263853379261E-2</c:v>
+                  <c:v>5.7660428128678859E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.23961405710699721</c:v>
+                  <c:v>0.14548239909522551</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4.6150407866800761E-3</c:v>
+                  <c:v>1.1277227894505011E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>0</c:v>
@@ -2847,34 +2856,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3.6301447953483071E-2</c:v>
+                  <c:v>3.7352310302486848E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>9.8988775407017907E-2</c:v>
+                  <c:v>4.7308621686181537E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.12761518648640241</c:v>
+                  <c:v>0.1069391968430348</c:v>
                 </c:pt>
                 <c:pt idx="45">
+                  <c:v>1.4775413711E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3.853598181563192E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.44764310943882E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.18069436235936789</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.2422654909378234</c:v>
+                </c:pt>
+                <c:pt idx="50">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="51">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>1.2005541018931819E-2</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.22877420893968639</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>9.7028995857734612E-2</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3381,28 +3390,28 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="0">
-                  <c:v>1.215813382424843E-2</c:v>
+                  <c:v>3.8589959309530972E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.06</c:v>
+                  <c:v>1.0538224179912639E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.8980063553496369E-2</c:v>
+                  <c:v>1.3210638502570021E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.6993620414673049E-2</c:v>
+                  <c:v>2.0431237471166239E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.1442326379736177E-2</c:v>
+                  <c:v>1.958613135973552E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.7936070872740336E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.7684128335224691E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -3411,13 +3420,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>1.619707790221173E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.5</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -3435,16 +3444,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>8.6772063237942773E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9.8942522132585854E-3</c:v>
+                  <c:v>9.855632961840716E-3</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>6.5371597438067114E-3</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0</c:v>
@@ -3474,13 +3483,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.206542658427171E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.16898698358800229</c:v>
+                  <c:v>5.6399721016769142E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.5253498611846558E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>0</c:v>
@@ -3492,10 +3501,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0</c:v>
+                  <c:v>1.3784632962010849E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0</c:v>
+                  <c:v>9.0926499434007563E-3</c:v>
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>0</c:v>
@@ -3510,10 +3519,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0</c:v>
+                  <c:v>1.774073313213767E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2.9807050356394889E-3</c:v>
+                  <c:v>2.8185502073370451E-3</c:v>
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>0</c:v>
@@ -3525,7 +3534,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.023622047244094E-2</c:v>
+                  <c:v>1.4235157418904489E-2</c:v>
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>0</c:v>
@@ -3534,7 +3543,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4036,160 +4045,160 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="0">
-                  <c:v>17.357636011930509</c:v>
+                  <c:v>14.335861002912781</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.95772233753641</c:v>
+                  <c:v>12.332954616955121</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31.624457308248921</c:v>
+                  <c:v>24.374095513748181</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19.7152403231756</c:v>
+                  <c:v>15.824208392410529</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17.574689971563132</c:v>
+                  <c:v>13.65554624509697</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25.124616475015131</c:v>
+                  <c:v>18.2067675568155</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.1742008859092543</c:v>
+                  <c:v>3.923657390340312</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13.70486221705503</c:v>
+                  <c:v>22.34768611469153</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16.024223047063821</c:v>
+                  <c:v>14.283581014273979</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.5</c:v>
+                  <c:v>2.4593775588215099</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16.25536628347373</c:v>
+                  <c:v>13.404402473732659</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>15.582271901687839</c:v>
+                  <c:v>12.93757435989837</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>34.299999999999997</c:v>
+                  <c:v>37.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.1826344708221583</c:v>
+                  <c:v>2.6087179420844322</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>10.250302306694691</c:v>
+                  <c:v>7.7765717707038151</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.8158248254329017</c:v>
+                  <c:v>7.6588278871291982</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.4658736792224958</c:v>
+                  <c:v>-1.384450435201467</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>14.566742228939111</c:v>
+                  <c:v>9.965282033109121</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>16.82400100506856</c:v>
+                  <c:v>14.75617730682297</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>25.73769718188154</c:v>
+                  <c:v>21.7053216764706</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>23.070834879406309</c:v>
+                  <c:v>19.460560678350468</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>16.51034553261092</c:v>
+                  <c:v>14.63957950216111</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>19.28738833420914</c:v>
+                  <c:v>18.97671352001991</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>14.67431458611803</c:v>
+                  <c:v>12.20021387668401</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>17.487872316126239</c:v>
+                  <c:v>14.389401862830541</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>18.427196859490021</c:v>
+                  <c:v>14.840330698529909</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>13.208016673240779</c:v>
+                  <c:v>9.6452059871731297</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>10.5</c:v>
+                  <c:v>-4.3</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>12.153526723670851</c:v>
+                  <c:v>7.8101154513315922</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>19.22843849235776</c:v>
+                  <c:v>15.42474054094588</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>19.169883120413161</c:v>
+                  <c:v>17.827272930030968</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>15.12231827805304</c:v>
+                  <c:v>13.849311605426429</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>24.105046380685451</c:v>
+                  <c:v>21.272202821169909</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>15.967946516271329</c:v>
+                  <c:v>17.229939550267979</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>25.134083170291341</c:v>
+                  <c:v>19.286998313900199</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>9.4168482349323614</c:v>
+                  <c:v>9.181666166164911</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>17.95838412263889</c:v>
+                  <c:v>14.18886933417409</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>16.02236399600573</c:v>
+                  <c:v>9.4882241286981639</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>15.10321619077502</c:v>
+                  <c:v>14.353629396060571</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>7.8922784668678059</c:v>
+                  <c:v>8.5449072661289698</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>16.3</c:v>
+                  <c:v>26.18</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>25.864164099237879</c:v>
+                  <c:v>19.94227693940185</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>12.065770739563</c:v>
+                  <c:v>11.89352908148301</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>16.239920481101759</c:v>
+                  <c:v>14.32148199852768</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>23.412296168591769</c:v>
+                  <c:v>15.51616555567329</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>8.5</c:v>
+                  <c:v>7.6736206812886687</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>17.456177606177611</c:v>
+                  <c:v>14.69061888465513</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>14.818362321071261</c:v>
+                  <c:v>14.799316817071601</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>13.90787401574803</c:v>
+                  <c:v>12.986598646276279</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>9.293469030474828</c:v>
+                  <c:v>8.7594407443505933</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>17.015772778239651</c:v>
+                  <c:v>10.8168676237062</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>10.7</c:v>
+                  <c:v>-4.1000000000000014</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4690,160 +4699,160 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="0">
-                  <c:v>25.639348425295971</c:v>
+                  <c:v>27.085007606792619</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.077796385151959</c:v>
+                  <c:v>19.70051821623181</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29.20410783055198</c:v>
+                  <c:v>30.872913992297811</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44.703116766429481</c:v>
+                  <c:v>49.972473747917661</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19.32809806519877</c:v>
+                  <c:v>18.777423104469211</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>34.700539860631508</c:v>
+                  <c:v>40.66359414337969</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23.44676164252364</c:v>
+                  <c:v>25.104965942977831</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21.825975615000441</c:v>
+                  <c:v>29.184664245367468</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>32.747340425156303</c:v>
+                  <c:v>30.814046297124261</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>30.3</c:v>
+                  <c:v>27.943122335534799</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>21.710974173962729</c:v>
+                  <c:v>22.053934071063431</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>27.062850271525509</c:v>
+                  <c:v>28.35371873369159</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>19.3</c:v>
+                  <c:v>20.8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>28.08996155462162</c:v>
+                  <c:v>29.495957896197918</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>27.389106468192661</c:v>
+                  <c:v>28.72107482689022</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>20.604587480983561</c:v>
+                  <c:v>21.177662917871341</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>21.42683628656782</c:v>
+                  <c:v>17.751867757529109</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>23.784716771955608</c:v>
+                  <c:v>24.327350727122461</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>19.179636481202579</c:v>
+                  <c:v>17.799402458622001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>23.16675632379987</c:v>
+                  <c:v>21.70910644580421</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>34.392838589981437</c:v>
+                  <c:v>34.865822417264233</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>29.718217133510532</c:v>
+                  <c:v>28.525247825675532</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>29.382448765107721</c:v>
+                  <c:v>33.597117135719351</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>22.200939289980699</c:v>
+                  <c:v>19.776313553338959</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24.447696616449321</c:v>
+                  <c:v>25.246048911796301</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>18.190324464273331</c:v>
+                  <c:v>13.297902088571741</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>21.971045484902969</c:v>
+                  <c:v>21.343614081599689</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>25.1</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>17.285995793276118</c:v>
+                  <c:v>26.396763341770871</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>29.893909081523219</c:v>
+                  <c:v>28.921658955041451</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>31.460940472954601</c:v>
+                  <c:v>32.214715571987497</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>27.394860582271988</c:v>
+                  <c:v>27.98871300604965</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>26.6759930811285</c:v>
+                  <c:v>32.311921812250773</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>22.023305601741701</c:v>
+                  <c:v>22.647336024162779</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>27.329493695275321</c:v>
+                  <c:v>25.877314550430061</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>19.98940201332854</c:v>
+                  <c:v>20.755435445477641</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>20.98393298820789</c:v>
+                  <c:v>17.515450672059512</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>16.97739899211965</c:v>
+                  <c:v>17.459591348152241</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>23.681801066834009</c:v>
+                  <c:v>24.78401561023605</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>20.703084143479721</c:v>
+                  <c:v>23.712841656234911</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>30.11</c:v>
+                  <c:v>23.08</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>29.244397600129719</c:v>
+                  <c:v>22.878868233520631</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>24.537035331729761</c:v>
+                  <c:v>24.422640481198389</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>23.673104387159071</c:v>
+                  <c:v>23.204049224603089</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>25.764683118276341</c:v>
+                  <c:v>33.20745361155906</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>23.8</c:v>
+                  <c:v>24.6651087614304</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>27.700514800514799</c:v>
+                  <c:v>29.713925743156981</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>26.457041711559182</c:v>
+                  <c:v>25.39026060144764</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>19.059055118110241</c:v>
+                  <c:v>19.352891181115279</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>17.16305998902822</c:v>
+                  <c:v>16.6044719089744</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>22.485768498788811</c:v>
+                  <c:v>19.278544196633732</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>14.4</c:v>
+                  <c:v>3.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9397,24 +9406,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M53"/>
+  <dimension ref="A1:M54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E8" sqref="E8"/>
+      <selection pane="topRight" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.83203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="39.83203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="38.5" style="3" customWidth="1"/>
-    <col min="5" max="5" width="40" style="3" customWidth="1"/>
-    <col min="6" max="6" width="36.5" style="3" customWidth="1"/>
-    <col min="7" max="7" width="42.1640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="46" style="3" customWidth="1"/>
-    <col min="9" max="9" width="44.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="34.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="31" style="3" customWidth="1"/>
+    <col min="4" max="4" width="27.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="27.83203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="29" style="3" customWidth="1"/>
+    <col min="8" max="8" width="33.33203125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="30.6640625" style="3" customWidth="1"/>
     <col min="10" max="13" width="18.83203125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9422,95 +9431,95 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
     </row>
-    <row r="2" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="14">
-        <v>17.357636011930509</v>
-      </c>
-      <c r="C2" s="14">
-        <v>7.182131594674444</v>
-      </c>
-      <c r="D2" s="14">
-        <v>25.639348425295971</v>
-      </c>
-      <c r="E2" s="14">
-        <v>0.92876007738819211</v>
-      </c>
-      <c r="F2" s="14">
-        <v>98.350445184713195</v>
-      </c>
-      <c r="G2" s="14">
-        <v>1.543912039881753</v>
-      </c>
-      <c r="H2" s="14">
-        <v>9.4010750793182093E-2</v>
-      </c>
-      <c r="I2" s="14">
-        <v>1.215813382424843E-2</v>
-      </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
+      <c r="B2" s="17">
+        <v>14.335861002912781</v>
+      </c>
+      <c r="C2" s="17">
+        <v>1.952226714230219</v>
+      </c>
+      <c r="D2" s="17">
+        <v>27.085007606792619</v>
+      </c>
+      <c r="E2" s="17">
+        <v>1.8816809396815011</v>
+      </c>
+      <c r="F2" s="17">
+        <v>98.448770971108942</v>
+      </c>
+      <c r="G2" s="17">
+        <v>1.4858257782428781</v>
+      </c>
+      <c r="H2" s="17">
+        <v>5.4600258989583497E-2</v>
+      </c>
+      <c r="I2" s="17">
+        <v>3.8589959309530972E-3</v>
+      </c>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="15">
-        <v>16.95772233753641</v>
-      </c>
-      <c r="C3" s="15">
-        <v>5.0699334977116646</v>
-      </c>
-      <c r="D3" s="15">
-        <v>21.077796385151959</v>
-      </c>
-      <c r="E3" s="15">
-        <v>-1.011871207653904</v>
-      </c>
-      <c r="F3" s="15">
-        <v>98.230449826989613</v>
-      </c>
-      <c r="G3" s="15">
-        <v>1.649550173010381</v>
-      </c>
-      <c r="H3" s="15">
-        <v>0.06</v>
-      </c>
-      <c r="I3" s="15">
-        <v>0.06</v>
+      <c r="B3" s="18">
+        <v>12.332954616955121</v>
+      </c>
+      <c r="C3" s="18">
+        <v>0.92173287444541352</v>
+      </c>
+      <c r="D3" s="18">
+        <v>19.70051821623181</v>
+      </c>
+      <c r="E3" s="18">
+        <v>-0.13684794955315249</v>
+      </c>
+      <c r="F3" s="18">
+        <v>99.12401472451748</v>
+      </c>
+      <c r="G3" s="18">
+        <v>0.79489501496721382</v>
+      </c>
+      <c r="H3" s="18">
+        <v>8.1090260514783491E-2</v>
+      </c>
+      <c r="I3" s="18">
+        <v>1.0538224179912639E-2</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
@@ -9521,28 +9530,28 @@
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="15">
-        <v>31.624457308248921</v>
-      </c>
-      <c r="C4" s="15">
-        <v>14.89704396159677</v>
-      </c>
-      <c r="D4" s="15">
-        <v>29.20410783055198</v>
-      </c>
-      <c r="E4" s="15">
-        <v>4.7891723060905722</v>
-      </c>
-      <c r="F4" s="15">
-        <v>99.428571428571431</v>
-      </c>
-      <c r="G4" s="15">
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="H4" s="15">
+      <c r="B4" s="18">
+        <v>24.374095513748181</v>
+      </c>
+      <c r="C4" s="18">
+        <v>1.6109009222038171</v>
+      </c>
+      <c r="D4" s="18">
+        <v>30.872913992297811</v>
+      </c>
+      <c r="E4" s="18">
+        <v>1.5944195316392571</v>
+      </c>
+      <c r="F4" s="18">
+        <v>99.714359906517785</v>
+      </c>
+      <c r="G4" s="18">
+        <v>0.28564009348221242</v>
+      </c>
+      <c r="H4" s="18">
         <v>0</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="18">
         <v>0</v>
       </c>
       <c r="J4" s="8"/>
@@ -9554,29 +9563,29 @@
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="15">
-        <v>19.7152403231756</v>
-      </c>
-      <c r="C5" s="15">
-        <v>9.4496423548841779</v>
-      </c>
-      <c r="D5" s="15">
-        <v>44.703116766429481</v>
-      </c>
-      <c r="E5" s="15">
-        <v>12.02115301407443</v>
-      </c>
-      <c r="F5" s="15">
-        <v>98.883536212467988</v>
-      </c>
-      <c r="G5" s="15">
-        <v>0.93095660003266567</v>
-      </c>
-      <c r="H5" s="15">
-        <v>0.15228198194286799</v>
-      </c>
-      <c r="I5" s="15">
-        <v>3.8980063553496369E-2</v>
+      <c r="B5" s="18">
+        <v>15.824208392410529</v>
+      </c>
+      <c r="C5" s="18">
+        <v>4.0428409707538684</v>
+      </c>
+      <c r="D5" s="18">
+        <v>49.972473747917661</v>
+      </c>
+      <c r="E5" s="18">
+        <v>1.8687629395474969</v>
+      </c>
+      <c r="F5" s="18">
+        <v>97.18399070433118</v>
+      </c>
+      <c r="G5" s="18">
+        <v>2.6258305484334659</v>
+      </c>
+      <c r="H5" s="18">
+        <v>0.17696810873265381</v>
+      </c>
+      <c r="I5" s="18">
+        <v>1.3210638502570021E-2</v>
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
@@ -9587,29 +9596,29 @@
       <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="15">
-        <v>17.574689971563132</v>
-      </c>
-      <c r="C6" s="15">
-        <v>6.6220640735251246</v>
-      </c>
-      <c r="D6" s="15">
-        <v>19.32809806519877</v>
-      </c>
-      <c r="E6" s="15">
-        <v>1.857241882840581</v>
-      </c>
-      <c r="F6" s="15">
-        <v>98.889434020073665</v>
-      </c>
-      <c r="G6" s="15">
-        <v>0.74903126015323229</v>
-      </c>
-      <c r="H6" s="15">
-        <v>0.36153471977310442</v>
-      </c>
-      <c r="I6" s="15">
-        <v>2.6993620414673049E-2</v>
+      <c r="B6" s="18">
+        <v>13.65554624509697</v>
+      </c>
+      <c r="C6" s="18">
+        <v>-0.3656504095981995</v>
+      </c>
+      <c r="D6" s="18">
+        <v>18.777423104469211</v>
+      </c>
+      <c r="E6" s="18">
+        <v>-0.21154512843720161</v>
+      </c>
+      <c r="F6" s="18">
+        <v>99.020743245283299</v>
+      </c>
+      <c r="G6" s="18">
+        <v>0.66645866145839117</v>
+      </c>
+      <c r="H6" s="18">
+        <v>0.29236685578686311</v>
+      </c>
+      <c r="I6" s="18">
+        <v>2.0431237471166239E-2</v>
       </c>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
@@ -9620,29 +9629,29 @@
       <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="15">
-        <v>25.124616475015131</v>
-      </c>
-      <c r="C7" s="15">
-        <v>8.8024638302302822</v>
-      </c>
-      <c r="D7" s="15">
-        <v>34.700539860631508</v>
-      </c>
-      <c r="E7" s="15">
-        <v>1.7554689761360209</v>
-      </c>
-      <c r="F7" s="15">
-        <v>94.474668190204341</v>
-      </c>
-      <c r="G7" s="15">
-        <v>5.3124914075953473</v>
-      </c>
-      <c r="H7" s="15">
-        <v>0.16139807582056881</v>
-      </c>
-      <c r="I7" s="15">
-        <v>5.1442326379736177E-2</v>
+      <c r="B7" s="18">
+        <v>18.2067675568155</v>
+      </c>
+      <c r="C7" s="18">
+        <v>1.066680421632493</v>
+      </c>
+      <c r="D7" s="18">
+        <v>40.66359414337969</v>
+      </c>
+      <c r="E7" s="18">
+        <v>4.9412887297431736</v>
+      </c>
+      <c r="F7" s="18">
+        <v>94.453619972606788</v>
+      </c>
+      <c r="G7" s="18">
+        <v>5.4751741780354184</v>
+      </c>
+      <c r="H7" s="18">
+        <v>6.9247236220964944E-2</v>
+      </c>
+      <c r="I7" s="18">
+        <v>1.958613135973552E-3</v>
       </c>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
@@ -9653,29 +9662,29 @@
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="15">
-        <v>6.1742008859092543</v>
-      </c>
-      <c r="C8" s="15">
-        <v>7.2351251047527834</v>
-      </c>
-      <c r="D8" s="15">
-        <v>23.44676164252364</v>
-      </c>
-      <c r="E8" s="15">
-        <v>-0.36619178738177888</v>
-      </c>
-      <c r="F8" s="15">
-        <v>97.348078534658214</v>
-      </c>
-      <c r="G8" s="15">
-        <v>2.6519214653417928</v>
-      </c>
-      <c r="H8" s="15">
+      <c r="B8" s="18">
+        <v>3.923657390340312</v>
+      </c>
+      <c r="C8" s="18">
+        <v>2.7416031909845779</v>
+      </c>
+      <c r="D8" s="18">
+        <v>25.104965942977831</v>
+      </c>
+      <c r="E8" s="18">
+        <v>0.97588659549228962</v>
+      </c>
+      <c r="F8" s="18">
+        <v>97.208349242055803</v>
+      </c>
+      <c r="G8" s="18">
+        <v>2.7850118794684779</v>
+      </c>
+      <c r="H8" s="18">
+        <v>6.6388784738578878E-3</v>
+      </c>
+      <c r="I8" s="18">
         <v>0</v>
-      </c>
-      <c r="I8" s="15">
-        <v>7.7936070872740336E-3</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
@@ -9686,29 +9695,29 @@
       <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="15">
-        <v>13.70486221705503</v>
-      </c>
-      <c r="C9" s="15">
-        <v>1.3082320607377189</v>
-      </c>
-      <c r="D9" s="15">
-        <v>21.825975615000441</v>
-      </c>
-      <c r="E9" s="15">
-        <v>-5.7728829523413498</v>
-      </c>
-      <c r="F9" s="15">
-        <v>98.633082109407638</v>
-      </c>
-      <c r="G9" s="15">
-        <v>1.194897111385903</v>
-      </c>
-      <c r="H9" s="15">
-        <v>0.1443366508712392</v>
-      </c>
-      <c r="I9" s="15">
-        <v>2.7684128335224691E-2</v>
+      <c r="B9" s="18">
+        <v>22.34768611469153</v>
+      </c>
+      <c r="C9" s="18">
+        <v>4.8722050297272528</v>
+      </c>
+      <c r="D9" s="18">
+        <v>29.184664245367468</v>
+      </c>
+      <c r="E9" s="18">
+        <v>2.2058329381210382</v>
+      </c>
+      <c r="F9" s="18">
+        <v>98.967191191276754</v>
+      </c>
+      <c r="G9" s="18">
+        <v>0.90535661506212473</v>
+      </c>
+      <c r="H9" s="18">
+        <v>0.12745219366051511</v>
+      </c>
+      <c r="I9" s="18">
+        <v>0</v>
       </c>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
@@ -9719,28 +9728,28 @@
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="15">
-        <v>16.024223047063821</v>
-      </c>
-      <c r="C10" s="15">
-        <v>7.5925392102399343</v>
-      </c>
-      <c r="D10" s="15">
-        <v>32.747340425156303</v>
-      </c>
-      <c r="E10" s="15">
-        <v>-0.30168700048458902</v>
-      </c>
-      <c r="F10" s="15">
-        <v>99.187185513388556</v>
-      </c>
-      <c r="G10" s="15">
-        <v>0.81281448661144307</v>
-      </c>
-      <c r="H10" s="15">
-        <v>8.7262569832402243E-2</v>
-      </c>
-      <c r="I10" s="15">
+      <c r="B10" s="18">
+        <v>14.283581014273979</v>
+      </c>
+      <c r="C10" s="18">
+        <v>1.824526569249975</v>
+      </c>
+      <c r="D10" s="18">
+        <v>30.814046297124261</v>
+      </c>
+      <c r="E10" s="18">
+        <v>-0.71507897940681897</v>
+      </c>
+      <c r="F10" s="18">
+        <v>98.954433270880301</v>
+      </c>
+      <c r="G10" s="18">
+        <v>1.0455667291188151</v>
+      </c>
+      <c r="H10" s="18">
+        <v>0</v>
+      </c>
+      <c r="I10" s="18">
         <v>0</v>
       </c>
       <c r="J10" s="8"/>
@@ -9752,28 +9761,28 @@
       <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="15">
-        <v>3.5</v>
-      </c>
-      <c r="C11" s="15">
-        <v>6.2</v>
-      </c>
-      <c r="D11" s="15">
-        <v>30.3</v>
-      </c>
-      <c r="E11" s="15">
-        <v>-1.8</v>
-      </c>
-      <c r="F11" s="15">
-        <v>98.7</v>
-      </c>
-      <c r="G11" s="15">
-        <v>1.3</v>
-      </c>
-      <c r="H11" s="15">
+      <c r="B11" s="18">
+        <v>2.4593775588215099</v>
+      </c>
+      <c r="C11" s="18">
+        <v>1.6867000000000001</v>
+      </c>
+      <c r="D11" s="18">
+        <v>27.943122335534799</v>
+      </c>
+      <c r="E11" s="18">
+        <v>-0.85229999999999995</v>
+      </c>
+      <c r="F11" s="18">
+        <v>99.292730844792999</v>
+      </c>
+      <c r="G11" s="18">
+        <v>0.70726915520599998</v>
+      </c>
+      <c r="H11" s="18">
         <v>0</v>
       </c>
-      <c r="I11" s="15">
+      <c r="I11" s="18">
         <v>0</v>
       </c>
       <c r="J11" s="8"/>
@@ -9785,29 +9794,29 @@
       <c r="A12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="15">
-        <v>16.25536628347373</v>
-      </c>
-      <c r="C12" s="15">
-        <v>5.678654475615569</v>
-      </c>
-      <c r="D12" s="15">
-        <v>21.710974173962729</v>
-      </c>
-      <c r="E12" s="15">
-        <v>0.10344826604216061</v>
-      </c>
-      <c r="F12" s="15">
-        <v>98.812390246711715</v>
-      </c>
-      <c r="G12" s="15">
-        <v>1.05778935659065</v>
-      </c>
-      <c r="H12" s="15">
-        <v>0.12982039669762999</v>
-      </c>
-      <c r="I12" s="15">
-        <v>0</v>
+      <c r="B12" s="18">
+        <v>13.404402473732659</v>
+      </c>
+      <c r="C12" s="18">
+        <v>3.6976566810100429</v>
+      </c>
+      <c r="D12" s="18">
+        <v>22.053934071063431</v>
+      </c>
+      <c r="E12" s="18">
+        <v>3.1007717736790998</v>
+      </c>
+      <c r="F12" s="18">
+        <v>98.917185071090771</v>
+      </c>
+      <c r="G12" s="18">
+        <v>1.006799081740112</v>
+      </c>
+      <c r="H12" s="18">
+        <v>7.6015847167901718E-2</v>
+      </c>
+      <c r="I12" s="18">
+        <v>1.619707790221173E-3</v>
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
@@ -9818,28 +9827,28 @@
       <c r="A13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="15">
-        <v>15.582271901687839</v>
-      </c>
-      <c r="C13" s="15">
-        <v>6.6333841407503211</v>
-      </c>
-      <c r="D13" s="15">
-        <v>27.062850271525509</v>
-      </c>
-      <c r="E13" s="15">
-        <v>0.87001695881590357</v>
-      </c>
-      <c r="F13" s="15">
-        <v>98.736350866274577</v>
-      </c>
-      <c r="G13" s="15">
-        <v>1.231103335617947</v>
-      </c>
-      <c r="H13" s="15">
-        <v>1.7870030189393812E-2</v>
-      </c>
-      <c r="I13" s="15">
+      <c r="B13" s="18">
+        <v>12.93757435989837</v>
+      </c>
+      <c r="C13" s="18">
+        <v>0.85765789170047335</v>
+      </c>
+      <c r="D13" s="18">
+        <v>28.35371873369159</v>
+      </c>
+      <c r="E13" s="18">
+        <v>1.2442931006904361</v>
+      </c>
+      <c r="F13" s="18">
+        <v>98.527046320812659</v>
+      </c>
+      <c r="G13" s="18">
+        <v>1.4543830932502031</v>
+      </c>
+      <c r="H13" s="18">
+        <v>3.8643254915559839E-3</v>
+      </c>
+      <c r="I13" s="18">
         <v>0</v>
       </c>
       <c r="J13" s="8"/>
@@ -9851,29 +9860,29 @@
       <c r="A14" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="15">
-        <v>34.299999999999997</v>
-      </c>
-      <c r="C14" s="15">
-        <v>-2.4</v>
-      </c>
-      <c r="D14" s="15">
-        <v>19.3</v>
-      </c>
-      <c r="E14" s="15">
-        <v>-1.4</v>
-      </c>
-      <c r="F14" s="15">
-        <v>94.199999999999989</v>
-      </c>
-      <c r="G14" s="15">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="H14" s="15">
-        <v>0.70000000000000007</v>
-      </c>
-      <c r="I14" s="15">
-        <v>0.5</v>
+      <c r="B14" s="18">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="C14" s="18">
+        <v>-3.5</v>
+      </c>
+      <c r="D14" s="18">
+        <v>20.8</v>
+      </c>
+      <c r="E14" s="18">
+        <v>1.4</v>
+      </c>
+      <c r="F14" s="18">
+        <v>97.2</v>
+      </c>
+      <c r="G14" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H14" s="18">
+        <v>0.2</v>
+      </c>
+      <c r="I14" s="18">
+        <v>0.1</v>
       </c>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
@@ -9884,28 +9893,28 @@
       <c r="A15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="15">
-        <v>4.1826344708221583</v>
-      </c>
-      <c r="C15" s="15">
-        <v>6.5897739721587323</v>
-      </c>
-      <c r="D15" s="15">
-        <v>28.08996155462162</v>
-      </c>
-      <c r="E15" s="15">
-        <v>1.445243494719439</v>
-      </c>
-      <c r="F15" s="15">
-        <v>99.855430846580589</v>
-      </c>
-      <c r="G15" s="15">
-        <v>0.1445691534194041</v>
-      </c>
-      <c r="H15" s="15">
+      <c r="B15" s="18">
+        <v>2.6087179420844322</v>
+      </c>
+      <c r="C15" s="18">
+        <v>0.90397531552482302</v>
+      </c>
+      <c r="D15" s="18">
+        <v>29.495957896197918</v>
+      </c>
+      <c r="E15" s="18">
+        <v>-0.51896038999611593</v>
+      </c>
+      <c r="F15" s="18">
+        <v>99.808514917536428</v>
+      </c>
+      <c r="G15" s="18">
+        <v>0.19148508246355911</v>
+      </c>
+      <c r="H15" s="18">
         <v>0</v>
       </c>
-      <c r="I15" s="15">
+      <c r="I15" s="18">
         <v>0</v>
       </c>
       <c r="J15" s="8"/>
@@ -9917,28 +9926,28 @@
       <c r="A16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="15">
-        <v>10.250302306694691</v>
-      </c>
-      <c r="C16" s="15">
-        <v>7.7061469513150129</v>
-      </c>
-      <c r="D16" s="15">
-        <v>27.389106468192661</v>
-      </c>
-      <c r="E16" s="15">
-        <v>9.4609577248970123E-2</v>
-      </c>
-      <c r="F16" s="15">
-        <v>99.33658330484306</v>
-      </c>
-      <c r="G16" s="15">
-        <v>0.66341669515695256</v>
-      </c>
-      <c r="H16" s="15">
+      <c r="B16" s="18">
+        <v>7.7765717707038151</v>
+      </c>
+      <c r="C16" s="18">
+        <v>1.084444709735864</v>
+      </c>
+      <c r="D16" s="18">
+        <v>28.72107482689022</v>
+      </c>
+      <c r="E16" s="18">
+        <v>2.059336055689327</v>
+      </c>
+      <c r="F16" s="18">
+        <v>99.291825730603719</v>
+      </c>
+      <c r="G16" s="18">
+        <v>0.70817426939542294</v>
+      </c>
+      <c r="H16" s="18">
         <v>0</v>
       </c>
-      <c r="I16" s="15">
+      <c r="I16" s="18">
         <v>0</v>
       </c>
       <c r="J16" s="8"/>
@@ -9950,28 +9959,28 @@
       <c r="A17" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="15">
-        <v>9.8158248254329017</v>
-      </c>
-      <c r="C17" s="15">
-        <v>6.0011892011473549</v>
-      </c>
-      <c r="D17" s="15">
-        <v>20.604587480983561</v>
-      </c>
-      <c r="E17" s="15">
-        <v>0.35862798818494018</v>
-      </c>
-      <c r="F17" s="15">
-        <v>99.518850414803154</v>
-      </c>
-      <c r="G17" s="15">
-        <v>0.48114958519685341</v>
-      </c>
-      <c r="H17" s="15">
-        <v>1.944228419064549E-2</v>
-      </c>
-      <c r="I17" s="15">
+      <c r="B17" s="18">
+        <v>7.6588278871291982</v>
+      </c>
+      <c r="C17" s="18">
+        <v>1.3155841759421401</v>
+      </c>
+      <c r="D17" s="18">
+        <v>21.177662917871341</v>
+      </c>
+      <c r="E17" s="18">
+        <v>1.3836458010305659</v>
+      </c>
+      <c r="F17" s="18">
+        <v>99.525914388943775</v>
+      </c>
+      <c r="G17" s="18">
+        <v>0.47408561105547931</v>
+      </c>
+      <c r="H17" s="18">
+        <v>0</v>
+      </c>
+      <c r="I17" s="18">
         <v>0</v>
       </c>
       <c r="J17" s="8"/>
@@ -9983,28 +9992,28 @@
       <c r="A18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="15">
-        <v>2.4658736792224958</v>
-      </c>
-      <c r="C18" s="15">
-        <v>5.1421627409326023</v>
-      </c>
-      <c r="D18" s="15">
-        <v>21.42683628656782</v>
-      </c>
-      <c r="E18" s="15">
-        <v>1.125743693918053</v>
-      </c>
-      <c r="F18" s="15">
-        <v>99.956930785824554</v>
-      </c>
-      <c r="G18" s="15">
-        <v>2.871280945030031E-2</v>
-      </c>
-      <c r="H18" s="15">
-        <v>1.435640472515015E-2</v>
-      </c>
-      <c r="I18" s="15">
+      <c r="B18" s="18">
+        <v>-1.384450435201467</v>
+      </c>
+      <c r="C18" s="18">
+        <v>-3.3857023090733802E-2</v>
+      </c>
+      <c r="D18" s="18">
+        <v>17.751867757529109</v>
+      </c>
+      <c r="E18" s="18">
+        <v>3.278806632706547</v>
+      </c>
+      <c r="F18" s="18">
+        <v>99.956238222437875</v>
+      </c>
+      <c r="G18" s="18">
+        <v>4.3761777562127832E-2</v>
+      </c>
+      <c r="H18" s="18">
+        <v>0</v>
+      </c>
+      <c r="I18" s="18">
         <v>0</v>
       </c>
       <c r="J18" s="8"/>
@@ -10016,28 +10025,28 @@
       <c r="A19" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="15">
-        <v>14.566742228939111</v>
-      </c>
-      <c r="C19" s="15">
-        <v>6.0556767927575361</v>
-      </c>
-      <c r="D19" s="15">
-        <v>23.784716771955608</v>
-      </c>
-      <c r="E19" s="15">
-        <v>0.18545035632577819</v>
-      </c>
-      <c r="F19" s="15">
-        <v>99.681635276898703</v>
-      </c>
-      <c r="G19" s="15">
-        <v>0.29804323719423093</v>
-      </c>
-      <c r="H19" s="15">
-        <v>2.0321485907049529E-2</v>
-      </c>
-      <c r="I19" s="15">
+      <c r="B19" s="18">
+        <v>9.965282033109121</v>
+      </c>
+      <c r="C19" s="18">
+        <v>1.1339414525998219</v>
+      </c>
+      <c r="D19" s="18">
+        <v>24.327350727122461</v>
+      </c>
+      <c r="E19" s="18">
+        <v>-0.44546958509614681</v>
+      </c>
+      <c r="F19" s="18">
+        <v>99.812933728801596</v>
+      </c>
+      <c r="G19" s="18">
+        <v>0.16688931933052881</v>
+      </c>
+      <c r="H19" s="18">
+        <v>2.0176951867881321E-2</v>
+      </c>
+      <c r="I19" s="18">
         <v>0</v>
       </c>
       <c r="J19" s="8"/>
@@ -10049,29 +10058,29 @@
       <c r="A20" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="15">
-        <v>16.82400100506856</v>
-      </c>
-      <c r="C20" s="15">
-        <v>5.6927302393753321</v>
-      </c>
-      <c r="D20" s="15">
-        <v>19.179636481202579</v>
-      </c>
-      <c r="E20" s="15">
-        <v>3.9921223457459658</v>
-      </c>
-      <c r="F20" s="15">
-        <v>98.791183744402119</v>
-      </c>
-      <c r="G20" s="15">
-        <v>1.101350177127197</v>
-      </c>
-      <c r="H20" s="15">
-        <v>0.10746607847069049</v>
-      </c>
-      <c r="I20" s="15">
-        <v>0</v>
+      <c r="B20" s="18">
+        <v>14.75617730682297</v>
+      </c>
+      <c r="C20" s="18">
+        <v>2.9471173091810901</v>
+      </c>
+      <c r="D20" s="18">
+        <v>17.799402458622001</v>
+      </c>
+      <c r="E20" s="18">
+        <v>-0.57083325002379515</v>
+      </c>
+      <c r="F20" s="18">
+        <v>98.896698018811293</v>
+      </c>
+      <c r="G20" s="18">
+        <v>1.006190380895204</v>
+      </c>
+      <c r="H20" s="18">
+        <v>1.033953705556667E-2</v>
+      </c>
+      <c r="I20" s="18">
+        <v>8.6772063237942773E-2</v>
       </c>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
@@ -10082,29 +10091,29 @@
       <c r="A21" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="15">
-        <v>25.73769718188154</v>
-      </c>
-      <c r="C21" s="15">
-        <v>4.2057078568512329</v>
-      </c>
-      <c r="D21" s="15">
-        <v>23.16675632379987</v>
-      </c>
-      <c r="E21" s="15">
-        <v>-0.70125557741213973</v>
-      </c>
-      <c r="F21" s="15">
-        <v>98.896033037690614</v>
-      </c>
-      <c r="G21" s="15">
-        <v>0.97615678214525847</v>
-      </c>
-      <c r="H21" s="15">
-        <v>0.1179159279508601</v>
-      </c>
-      <c r="I21" s="15">
-        <v>9.8942522132585854E-3</v>
+      <c r="B21" s="18">
+        <v>21.7053216764706</v>
+      </c>
+      <c r="C21" s="18">
+        <v>1.698513515310103</v>
+      </c>
+      <c r="D21" s="18">
+        <v>21.70910644580421</v>
+      </c>
+      <c r="E21" s="18">
+        <v>-0.62481056998156903</v>
+      </c>
+      <c r="F21" s="18">
+        <v>99.231690431672376</v>
+      </c>
+      <c r="G21" s="18">
+        <v>0.63260642698065905</v>
+      </c>
+      <c r="H21" s="18">
+        <v>0.12584750838499581</v>
+      </c>
+      <c r="I21" s="18">
+        <v>9.855632961840716E-3</v>
       </c>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
@@ -10115,28 +10124,28 @@
       <c r="A22" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="15">
-        <v>23.070834879406309</v>
-      </c>
-      <c r="C22" s="15">
-        <v>9.606641929499073</v>
-      </c>
-      <c r="D22" s="15">
-        <v>34.392838589981437</v>
-      </c>
-      <c r="E22" s="15">
-        <v>2.6493506493506498</v>
-      </c>
-      <c r="F22" s="15">
-        <v>99.678515769944354</v>
-      </c>
-      <c r="G22" s="15">
-        <v>0.32148423005565863</v>
-      </c>
-      <c r="H22" s="15">
+      <c r="B22" s="18">
+        <v>19.460560678350468</v>
+      </c>
+      <c r="C22" s="18">
+        <v>3.5139095255744999</v>
+      </c>
+      <c r="D22" s="18">
+        <v>34.865822417264233</v>
+      </c>
+      <c r="E22" s="18">
+        <v>2.3920596738324691</v>
+      </c>
+      <c r="F22" s="18">
+        <v>99.699584356290615</v>
+      </c>
+      <c r="G22" s="18">
+        <v>0.30041564370931401</v>
+      </c>
+      <c r="H22" s="18">
         <v>0</v>
       </c>
-      <c r="I22" s="15">
+      <c r="I22" s="18">
         <v>0</v>
       </c>
       <c r="J22" s="8"/>
@@ -10148,29 +10157,29 @@
       <c r="A23" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="15">
-        <v>16.51034553261092</v>
-      </c>
-      <c r="C23" s="15">
-        <v>7.5012369658556528</v>
-      </c>
-      <c r="D23" s="15">
-        <v>29.718217133510532</v>
-      </c>
-      <c r="E23" s="15">
-        <v>9.561439378450215E-2</v>
-      </c>
-      <c r="F23" s="15">
-        <v>98.994827233694537</v>
-      </c>
-      <c r="G23" s="15">
-        <v>1.005172766305459</v>
-      </c>
-      <c r="H23" s="15">
-        <v>0</v>
-      </c>
-      <c r="I23" s="15">
-        <v>0</v>
+      <c r="B23" s="18">
+        <v>14.63957950216111</v>
+      </c>
+      <c r="C23" s="18">
+        <v>1.7200992758057929</v>
+      </c>
+      <c r="D23" s="18">
+        <v>28.525247825675532</v>
+      </c>
+      <c r="E23" s="18">
+        <v>-0.35240948592411259</v>
+      </c>
+      <c r="F23" s="18">
+        <v>99.261300948858931</v>
+      </c>
+      <c r="G23" s="18">
+        <v>0.7125504121618339</v>
+      </c>
+      <c r="H23" s="18">
+        <v>2.614863897822348E-2</v>
+      </c>
+      <c r="I23" s="18">
+        <v>6.5371597438067114E-3</v>
       </c>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
@@ -10181,28 +10190,28 @@
       <c r="A24" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="15">
-        <v>19.28738833420914</v>
-      </c>
-      <c r="C24" s="15">
-        <v>9.6141355754072517</v>
-      </c>
-      <c r="D24" s="15">
-        <v>29.382448765107721</v>
-      </c>
-      <c r="E24" s="15">
-        <v>0.31823436678928008</v>
-      </c>
-      <c r="F24" s="15">
-        <v>98.942249080399378</v>
-      </c>
-      <c r="G24" s="15">
-        <v>0.96831318970047298</v>
-      </c>
-      <c r="H24" s="15">
-        <v>8.943772990015765E-2</v>
-      </c>
-      <c r="I24" s="15">
+      <c r="B24" s="18">
+        <v>18.97671352001991</v>
+      </c>
+      <c r="C24" s="18">
+        <v>4.5705902515723276</v>
+      </c>
+      <c r="D24" s="18">
+        <v>33.597117135719351</v>
+      </c>
+      <c r="E24" s="18">
+        <v>1.976588836477988</v>
+      </c>
+      <c r="F24" s="18">
+        <v>99.203435916753321</v>
+      </c>
+      <c r="G24" s="18">
+        <v>0.69948790181621534</v>
+      </c>
+      <c r="H24" s="18">
+        <v>9.7076181428672956E-2</v>
+      </c>
+      <c r="I24" s="18">
         <v>0</v>
       </c>
       <c r="J24" s="8"/>
@@ -10214,28 +10223,28 @@
       <c r="A25" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="15">
-        <v>14.67431458611803</v>
-      </c>
-      <c r="C25" s="15">
-        <v>7.6909690090531244</v>
-      </c>
-      <c r="D25" s="15">
-        <v>22.200939289980699</v>
-      </c>
-      <c r="E25" s="15">
-        <v>-0.46805123518739628</v>
-      </c>
-      <c r="F25" s="15">
-        <v>99.605794465376121</v>
-      </c>
-      <c r="G25" s="15">
-        <v>0.32568533194751198</v>
-      </c>
-      <c r="H25" s="15">
+      <c r="B25" s="18">
+        <v>12.20021387668401</v>
+      </c>
+      <c r="C25" s="18">
+        <v>2.853976959114358</v>
+      </c>
+      <c r="D25" s="18">
+        <v>19.776313553338959</v>
+      </c>
+      <c r="E25" s="18">
+        <v>0.90560901382307935</v>
+      </c>
+      <c r="F25" s="18">
+        <v>99.828981233949207</v>
+      </c>
+      <c r="G25" s="18">
+        <v>0.17101876605010141</v>
+      </c>
+      <c r="H25" s="18">
         <v>0</v>
       </c>
-      <c r="I25" s="15">
+      <c r="I25" s="18">
         <v>0</v>
       </c>
       <c r="J25" s="8"/>
@@ -10247,28 +10256,28 @@
       <c r="A26" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="15">
-        <v>17.487872316126239</v>
-      </c>
-      <c r="C26" s="15">
-        <v>8.0977583580367547</v>
-      </c>
-      <c r="D26" s="15">
-        <v>24.447696616449321</v>
-      </c>
-      <c r="E26" s="15">
-        <v>0.34735147219181878</v>
-      </c>
-      <c r="F26" s="15">
-        <v>99.325396889801894</v>
-      </c>
-      <c r="G26" s="15">
-        <v>0.6067087236882186</v>
-      </c>
-      <c r="H26" s="15">
-        <v>6.7894386509873533E-2</v>
-      </c>
-      <c r="I26" s="15">
+      <c r="B26" s="18">
+        <v>14.389401862830541</v>
+      </c>
+      <c r="C26" s="18">
+        <v>-0.35076249485863709</v>
+      </c>
+      <c r="D26" s="18">
+        <v>25.246048911796301</v>
+      </c>
+      <c r="E26" s="18">
+        <v>-0.2130501858234348</v>
+      </c>
+      <c r="F26" s="18">
+        <v>99.52805889864625</v>
+      </c>
+      <c r="G26" s="18">
+        <v>0.44598518800130649</v>
+      </c>
+      <c r="H26" s="18">
+        <v>2.5955913351755601E-2</v>
+      </c>
+      <c r="I26" s="18">
         <v>0</v>
       </c>
       <c r="J26" s="8"/>
@@ -10280,28 +10289,28 @@
       <c r="A27" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="15">
-        <v>18.427196859490021</v>
-      </c>
-      <c r="C27" s="15">
-        <v>4.2454046893045598</v>
-      </c>
-      <c r="D27" s="15">
-        <v>18.190324464273331</v>
-      </c>
-      <c r="E27" s="15">
-        <v>1.407137606983017</v>
-      </c>
-      <c r="F27" s="15">
-        <v>99.309816037517152</v>
-      </c>
-      <c r="G27" s="15">
-        <v>0.62082116043099922</v>
-      </c>
-      <c r="H27" s="15">
-        <v>6.9362802051866346E-2</v>
-      </c>
-      <c r="I27" s="15">
+      <c r="B27" s="18">
+        <v>14.840330698529909</v>
+      </c>
+      <c r="C27" s="18">
+        <v>-0.6715656589898179</v>
+      </c>
+      <c r="D27" s="18">
+        <v>13.297902088571741</v>
+      </c>
+      <c r="E27" s="18">
+        <v>-2.6188696749271898</v>
+      </c>
+      <c r="F27" s="18">
+        <v>99.672612942989701</v>
+      </c>
+      <c r="G27" s="18">
+        <v>0.28818617965387272</v>
+      </c>
+      <c r="H27" s="18">
+        <v>3.9200877355929697E-2</v>
+      </c>
+      <c r="I27" s="18">
         <v>0</v>
       </c>
       <c r="J27" s="8"/>
@@ -10313,28 +10322,28 @@
       <c r="A28" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="15">
-        <v>13.208016673240779</v>
-      </c>
-      <c r="C28" s="15">
-        <v>5.0925920537711651</v>
-      </c>
-      <c r="D28" s="15">
-        <v>21.971045484902969</v>
-      </c>
-      <c r="E28" s="15">
-        <v>0.128222826480554</v>
-      </c>
-      <c r="F28" s="15">
-        <v>98.888043074107941</v>
-      </c>
-      <c r="G28" s="15">
-        <v>1.081573410826616</v>
-      </c>
-      <c r="H28" s="15">
-        <v>3.0383515065444039E-2</v>
-      </c>
-      <c r="I28" s="15">
+      <c r="B28" s="18">
+        <v>9.6452059871731297</v>
+      </c>
+      <c r="C28" s="18">
+        <v>3.6997261891173798E-2</v>
+      </c>
+      <c r="D28" s="18">
+        <v>21.343614081599689</v>
+      </c>
+      <c r="E28" s="18">
+        <v>0.18811453368439379</v>
+      </c>
+      <c r="F28" s="18">
+        <v>99.124717048391474</v>
+      </c>
+      <c r="G28" s="18">
+        <v>0.86012890175247969</v>
+      </c>
+      <c r="H28" s="18">
+        <v>1.5154049855972679E-2</v>
+      </c>
+      <c r="I28" s="18">
         <v>0</v>
       </c>
       <c r="J28" s="8"/>
@@ -10346,28 +10355,28 @@
       <c r="A29" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="15">
-        <v>10.5</v>
-      </c>
-      <c r="C29" s="15">
-        <v>8.1</v>
-      </c>
-      <c r="D29" s="15">
-        <v>25.1</v>
-      </c>
-      <c r="E29" s="15">
-        <v>5.2</v>
-      </c>
-      <c r="F29" s="15">
-        <v>98.6</v>
-      </c>
-      <c r="G29" s="15">
-        <v>1.3</v>
-      </c>
-      <c r="H29" s="15">
+      <c r="B29" s="18">
+        <v>-4.3</v>
+      </c>
+      <c r="C29" s="18">
+        <v>-9.1</v>
+      </c>
+      <c r="D29" s="18">
+        <v>9</v>
+      </c>
+      <c r="E29" s="18">
+        <v>-12.4</v>
+      </c>
+      <c r="F29" s="18">
+        <v>99</v>
+      </c>
+      <c r="G29" s="18">
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="H29" s="18">
         <v>0</v>
       </c>
-      <c r="I29" s="15">
+      <c r="I29" s="18">
         <v>0</v>
       </c>
       <c r="J29" s="8"/>
@@ -10379,28 +10388,28 @@
       <c r="A30" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="15">
-        <v>12.153526723670851</v>
-      </c>
-      <c r="C30" s="15">
-        <v>2.8211160073263648</v>
-      </c>
-      <c r="D30" s="15">
-        <v>17.285995793276118</v>
-      </c>
-      <c r="E30" s="15">
-        <v>0.55734966971934485</v>
-      </c>
-      <c r="F30" s="15">
-        <v>99.94009681323115</v>
-      </c>
-      <c r="G30" s="15">
-        <v>5.9903186768858412E-2</v>
-      </c>
-      <c r="H30" s="15">
+      <c r="B30" s="18">
+        <v>7.8101154513315922</v>
+      </c>
+      <c r="C30" s="18">
+        <v>2.3594707781631499</v>
+      </c>
+      <c r="D30" s="18">
+        <v>26.396763341770871</v>
+      </c>
+      <c r="E30" s="18">
+        <v>5.517907403754454</v>
+      </c>
+      <c r="F30" s="18">
+        <v>99.411656614394857</v>
+      </c>
+      <c r="G30" s="18">
+        <v>0.58834338560514676</v>
+      </c>
+      <c r="H30" s="18">
         <v>0</v>
       </c>
-      <c r="I30" s="15">
+      <c r="I30" s="18">
         <v>0</v>
       </c>
       <c r="J30" s="8"/>
@@ -10412,28 +10421,28 @@
       <c r="A31" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="15">
-        <v>19.22843849235776</v>
-      </c>
-      <c r="C31" s="15">
-        <v>6.8730564758989017</v>
-      </c>
-      <c r="D31" s="15">
-        <v>29.893909081523219</v>
-      </c>
-      <c r="E31" s="15">
-        <v>4.7747896778307144</v>
-      </c>
-      <c r="F31" s="15">
-        <v>98.857015003948405</v>
-      </c>
-      <c r="G31" s="15">
-        <v>1.0604764411687291</v>
-      </c>
-      <c r="H31" s="15">
-        <v>8.2508554882863905E-2</v>
-      </c>
-      <c r="I31" s="15">
+      <c r="B31" s="18">
+        <v>15.42474054094588</v>
+      </c>
+      <c r="C31" s="18">
+        <v>3.656372797142176</v>
+      </c>
+      <c r="D31" s="18">
+        <v>28.921658955041451</v>
+      </c>
+      <c r="E31" s="18">
+        <v>2.3116607333001529</v>
+      </c>
+      <c r="F31" s="18">
+        <v>98.886108176100635</v>
+      </c>
+      <c r="G31" s="18">
+        <v>1.015059119496855</v>
+      </c>
+      <c r="H31" s="18">
+        <v>7.0631446540880508E-2</v>
+      </c>
+      <c r="I31" s="18">
         <v>0</v>
       </c>
       <c r="J31" s="8"/>
@@ -10445,28 +10454,28 @@
       <c r="A32" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="15">
-        <v>19.169883120413161</v>
-      </c>
-      <c r="C32" s="15">
-        <v>9.9847512911117153</v>
-      </c>
-      <c r="D32" s="15">
-        <v>31.460940472954601</v>
-      </c>
-      <c r="E32" s="15">
-        <v>0.84240282685512369</v>
-      </c>
-      <c r="F32" s="15">
-        <v>99.524245718945366</v>
-      </c>
-      <c r="G32" s="15">
-        <v>0.47575428105463441</v>
-      </c>
-      <c r="H32" s="15">
-        <v>0</v>
-      </c>
-      <c r="I32" s="15">
+      <c r="B32" s="18">
+        <v>17.827272930030968</v>
+      </c>
+      <c r="C32" s="18">
+        <v>3.901217438396968</v>
+      </c>
+      <c r="D32" s="18">
+        <v>32.214715571987497</v>
+      </c>
+      <c r="E32" s="18">
+        <v>1.4834379637151369</v>
+      </c>
+      <c r="F32" s="18">
+        <v>99.570509081207035</v>
+      </c>
+      <c r="G32" s="18">
+        <v>0.38086996142046031</v>
+      </c>
+      <c r="H32" s="18">
+        <v>4.8620957370760901E-2</v>
+      </c>
+      <c r="I32" s="18">
         <v>0</v>
       </c>
       <c r="J32" s="8"/>
@@ -10478,29 +10487,29 @@
       <c r="A33" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="15">
-        <v>15.12231827805304</v>
-      </c>
-      <c r="C33" s="15">
-        <v>7.1051307974837261</v>
-      </c>
-      <c r="D33" s="15">
-        <v>27.394860582271988</v>
-      </c>
-      <c r="E33" s="15">
-        <v>-1.9344101441374619</v>
-      </c>
-      <c r="F33" s="15">
-        <v>98.549879049470803</v>
-      </c>
-      <c r="G33" s="15">
-        <v>1.379577012043796</v>
-      </c>
-      <c r="H33" s="15">
-        <v>6.7337395826970597E-2</v>
-      </c>
-      <c r="I33" s="15">
-        <v>3.206542658427171E-3</v>
+      <c r="B33" s="18">
+        <v>13.849311605426429</v>
+      </c>
+      <c r="C33" s="18">
+        <v>1.7557482065236309</v>
+      </c>
+      <c r="D33" s="18">
+        <v>27.98871300604965</v>
+      </c>
+      <c r="E33" s="18">
+        <v>-0.27577313300434431</v>
+      </c>
+      <c r="F33" s="18">
+        <v>98.891262814515713</v>
+      </c>
+      <c r="G33" s="18">
+        <v>1.0576684818707771</v>
+      </c>
+      <c r="H33" s="18">
+        <v>5.1068703612935633E-2</v>
+      </c>
+      <c r="I33" s="18">
+        <v>0</v>
       </c>
       <c r="J33" s="8"/>
       <c r="K33" s="8"/>
@@ -10511,29 +10520,29 @@
       <c r="A34" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="15">
-        <v>24.105046380685451</v>
-      </c>
-      <c r="C34" s="15">
-        <v>8.3164511095824363</v>
-      </c>
-      <c r="D34" s="15">
-        <v>26.6759930811285</v>
-      </c>
-      <c r="E34" s="15">
-        <v>1.210525191929757</v>
-      </c>
-      <c r="F34" s="15">
-        <v>97.676327851540989</v>
-      </c>
-      <c r="G34" s="15">
-        <v>1.953987840829263</v>
-      </c>
-      <c r="H34" s="15">
-        <v>0.36968430762975069</v>
-      </c>
-      <c r="I34" s="15">
-        <v>0.16898698358800229</v>
+      <c r="B34" s="18">
+        <v>21.272202821169909</v>
+      </c>
+      <c r="C34" s="18">
+        <v>1.345882270796938</v>
+      </c>
+      <c r="D34" s="18">
+        <v>32.311921812250773</v>
+      </c>
+      <c r="E34" s="18">
+        <v>2.9888207865388789</v>
+      </c>
+      <c r="F34" s="18">
+        <v>97.36805139451937</v>
+      </c>
+      <c r="G34" s="18">
+        <v>2.4032291953466012</v>
+      </c>
+      <c r="H34" s="18">
+        <v>0.22871941013318581</v>
+      </c>
+      <c r="I34" s="18">
+        <v>5.6399721016769142E-2</v>
       </c>
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
@@ -10544,29 +10553,29 @@
       <c r="A35" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B35" s="15">
-        <v>15.967946516271329</v>
-      </c>
-      <c r="C35" s="15">
-        <v>6.6621963030695772</v>
-      </c>
-      <c r="D35" s="15">
-        <v>22.023305601741701</v>
-      </c>
-      <c r="E35" s="15">
-        <v>1.423310368769088</v>
-      </c>
-      <c r="F35" s="15">
-        <v>98.689506575357768</v>
-      </c>
-      <c r="G35" s="15">
-        <v>1.220446568705549</v>
-      </c>
-      <c r="H35" s="15">
-        <v>8.6521506075509638E-2</v>
-      </c>
-      <c r="I35" s="15">
-        <v>3.5253498611846558E-3</v>
+      <c r="B35" s="18">
+        <v>17.229939550267979</v>
+      </c>
+      <c r="C35" s="18">
+        <v>4.6367042716560203</v>
+      </c>
+      <c r="D35" s="18">
+        <v>22.647336024162779</v>
+      </c>
+      <c r="E35" s="18">
+        <v>1.882629026883506</v>
+      </c>
+      <c r="F35" s="18">
+        <v>98.879490816348465</v>
+      </c>
+      <c r="G35" s="18">
+        <v>1.0208197090178961</v>
+      </c>
+      <c r="H35" s="18">
+        <v>3.9378977358205468E-2</v>
+      </c>
+      <c r="I35" s="18">
+        <v>0</v>
       </c>
       <c r="J35" s="8"/>
       <c r="K35" s="8"/>
@@ -10577,28 +10586,28 @@
       <c r="A36" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B36" s="15">
-        <v>25.134083170291341</v>
-      </c>
-      <c r="C36" s="15">
-        <v>9.543301673887477</v>
-      </c>
-      <c r="D36" s="15">
-        <v>27.329493695275321</v>
-      </c>
-      <c r="E36" s="15">
-        <v>5.1958867938428996</v>
-      </c>
-      <c r="F36" s="15">
-        <v>98.443899287680551</v>
-      </c>
-      <c r="G36" s="15">
-        <v>1.46118949031643</v>
-      </c>
-      <c r="H36" s="15">
-        <v>9.4911222003017298E-2</v>
-      </c>
-      <c r="I36" s="15">
+      <c r="B36" s="18">
+        <v>19.286998313900199</v>
+      </c>
+      <c r="C36" s="18">
+        <v>-2.512053672974583</v>
+      </c>
+      <c r="D36" s="18">
+        <v>25.877314550430061</v>
+      </c>
+      <c r="E36" s="18">
+        <v>1.865211027121678</v>
+      </c>
+      <c r="F36" s="18">
+        <v>98.637052844204064</v>
+      </c>
+      <c r="G36" s="18">
+        <v>1.264622817443823</v>
+      </c>
+      <c r="H36" s="18">
+        <v>3.3983952833643782E-3</v>
+      </c>
+      <c r="I36" s="18">
         <v>0</v>
       </c>
       <c r="J36" s="8"/>
@@ -10610,28 +10619,28 @@
       <c r="A37" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B37" s="15">
-        <v>9.4168482349323614</v>
-      </c>
-      <c r="C37" s="15">
-        <v>3.8390158737684938</v>
-      </c>
-      <c r="D37" s="15">
-        <v>19.98940201332854</v>
-      </c>
-      <c r="E37" s="15">
-        <v>1.917205337632232</v>
-      </c>
-      <c r="F37" s="15">
-        <v>99.97220991615103</v>
-      </c>
-      <c r="G37" s="15">
-        <v>2.7790083848971241E-2</v>
-      </c>
-      <c r="H37" s="15">
+      <c r="B37" s="18">
+        <v>9.181666166164911</v>
+      </c>
+      <c r="C37" s="18">
+        <v>-0.41384953209198372</v>
+      </c>
+      <c r="D37" s="18">
+        <v>20.755435445477641</v>
+      </c>
+      <c r="E37" s="18">
+        <v>-0.51352497947364284</v>
+      </c>
+      <c r="F37" s="18">
+        <v>100</v>
+      </c>
+      <c r="G37" s="18">
         <v>0</v>
       </c>
-      <c r="I37" s="15">
+      <c r="H37" s="18">
+        <v>0</v>
+      </c>
+      <c r="I37" s="18">
         <v>0</v>
       </c>
       <c r="J37" s="8"/>
@@ -10643,28 +10652,28 @@
       <c r="A38" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B38" s="15">
-        <v>17.95838412263889</v>
-      </c>
-      <c r="C38" s="15">
-        <v>5.5037833564203051</v>
-      </c>
-      <c r="D38" s="15">
-        <v>20.98393298820789</v>
-      </c>
-      <c r="E38" s="15">
-        <v>3.5845977602382462</v>
-      </c>
-      <c r="F38" s="15">
-        <v>98.895123459400367</v>
-      </c>
-      <c r="G38" s="15">
-        <v>1.002256900715857</v>
-      </c>
-      <c r="H38" s="15">
-        <v>0.1026196398837813</v>
-      </c>
-      <c r="I38" s="15">
+      <c r="B38" s="18">
+        <v>14.18886933417409</v>
+      </c>
+      <c r="C38" s="18">
+        <v>3.4079576584502052</v>
+      </c>
+      <c r="D38" s="18">
+        <v>17.515450672059512</v>
+      </c>
+      <c r="E38" s="18">
+        <v>-0.3830916636220083</v>
+      </c>
+      <c r="F38" s="18">
+        <v>99.28012133043336</v>
+      </c>
+      <c r="G38" s="18">
+        <v>0.69851521178124309</v>
+      </c>
+      <c r="H38" s="18">
+        <v>2.136345778536302E-2</v>
+      </c>
+      <c r="I38" s="18">
         <v>0</v>
       </c>
       <c r="J38" s="8"/>
@@ -10676,29 +10685,29 @@
       <c r="A39" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B39" s="15">
-        <v>16.02236399600573</v>
-      </c>
-      <c r="C39" s="15">
-        <v>8.5871894165134908</v>
-      </c>
-      <c r="D39" s="15">
-        <v>16.97739899211965</v>
-      </c>
-      <c r="E39" s="15">
-        <v>0.50105294508293641</v>
-      </c>
-      <c r="F39" s="15">
-        <v>99.739367282263643</v>
-      </c>
-      <c r="G39" s="15">
-        <v>0.24594845388298159</v>
-      </c>
-      <c r="H39" s="15">
-        <v>1.4684263853379261E-2</v>
-      </c>
-      <c r="I39" s="15">
-        <v>0</v>
+      <c r="B39" s="18">
+        <v>9.4882241286981639</v>
+      </c>
+      <c r="C39" s="18">
+        <v>1.983040472960746</v>
+      </c>
+      <c r="D39" s="18">
+        <v>17.459591348152241</v>
+      </c>
+      <c r="E39" s="18">
+        <v>0.60589875885424127</v>
+      </c>
+      <c r="F39" s="18">
+        <v>99.645264215408531</v>
+      </c>
+      <c r="G39" s="18">
+        <v>0.28329072350077578</v>
+      </c>
+      <c r="H39" s="18">
+        <v>5.7660428128678859E-2</v>
+      </c>
+      <c r="I39" s="18">
+        <v>1.3784632962010849E-2</v>
       </c>
       <c r="J39" s="8"/>
       <c r="K39" s="8"/>
@@ -10709,29 +10718,29 @@
       <c r="A40" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B40" s="15">
-        <v>15.10321619077502</v>
-      </c>
-      <c r="C40" s="15">
-        <v>8.9987135236899913</v>
-      </c>
-      <c r="D40" s="15">
-        <v>23.681801066834009</v>
-      </c>
-      <c r="E40" s="15">
-        <v>0.76167241920301221</v>
-      </c>
-      <c r="F40" s="15">
-        <v>98.679871352369005</v>
-      </c>
-      <c r="G40" s="15">
-        <v>1.0805145905240039</v>
-      </c>
-      <c r="H40" s="15">
-        <v>0.23961405710699721</v>
-      </c>
-      <c r="I40" s="15">
-        <v>0</v>
+      <c r="B40" s="18">
+        <v>14.353629396060571</v>
+      </c>
+      <c r="C40" s="18">
+        <v>4.0209003783698556</v>
+      </c>
+      <c r="D40" s="18">
+        <v>24.78401561023605</v>
+      </c>
+      <c r="E40" s="18">
+        <v>0.79869746176887924</v>
+      </c>
+      <c r="F40" s="18">
+        <v>98.842347778967309</v>
+      </c>
+      <c r="G40" s="18">
+        <v>1.0121698219366579</v>
+      </c>
+      <c r="H40" s="18">
+        <v>0.14548239909522551</v>
+      </c>
+      <c r="I40" s="18">
+        <v>9.0926499434007563E-3</v>
       </c>
       <c r="J40" s="8"/>
       <c r="K40" s="8"/>
@@ -10742,28 +10751,28 @@
       <c r="A41" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B41" s="15">
-        <v>7.8922784668678059</v>
-      </c>
-      <c r="C41" s="15">
-        <v>8.2138451223600395</v>
-      </c>
-      <c r="D41" s="15">
-        <v>20.703084143479721</v>
-      </c>
-      <c r="E41" s="15">
-        <v>0.1015085484411667</v>
-      </c>
-      <c r="F41" s="15">
-        <v>99.467694714493234</v>
-      </c>
-      <c r="G41" s="15">
-        <v>0.52769024472008041</v>
-      </c>
-      <c r="H41" s="15">
-        <v>4.6150407866800761E-3</v>
-      </c>
-      <c r="I41" s="15">
+      <c r="B41" s="18">
+        <v>8.5449072661289698</v>
+      </c>
+      <c r="C41" s="18">
+        <v>3.2707898537226758</v>
+      </c>
+      <c r="D41" s="18">
+        <v>23.712841656234911</v>
+      </c>
+      <c r="E41" s="18">
+        <v>1.232272042951843</v>
+      </c>
+      <c r="F41" s="18">
+        <v>99.494973882957183</v>
+      </c>
+      <c r="G41" s="18">
+        <v>0.49374888914639692</v>
+      </c>
+      <c r="H41" s="18">
+        <v>1.1277227894505011E-2</v>
+      </c>
+      <c r="I41" s="18">
         <v>0</v>
       </c>
       <c r="J41" s="8"/>
@@ -10775,28 +10784,28 @@
       <c r="A42" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B42" s="15">
-        <v>16.3</v>
-      </c>
-      <c r="C42" s="15">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="D42" s="15">
-        <v>30.11</v>
-      </c>
-      <c r="E42" s="15">
-        <v>7.3999999999999986</v>
-      </c>
-      <c r="F42" s="15">
-        <v>99.86</v>
-      </c>
-      <c r="G42" s="15">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="H42" s="15">
+      <c r="B42" s="18">
+        <v>26.18</v>
+      </c>
+      <c r="C42" s="18">
+        <v>8.7900000000000009</v>
+      </c>
+      <c r="D42" s="18">
+        <v>23.08</v>
+      </c>
+      <c r="E42" s="18">
+        <v>0.36</v>
+      </c>
+      <c r="F42" s="18">
+        <v>99.76</v>
+      </c>
+      <c r="G42" s="18">
+        <v>0.24</v>
+      </c>
+      <c r="H42" s="18">
         <v>0</v>
       </c>
-      <c r="I42" s="15">
+      <c r="I42" s="18">
         <v>0</v>
       </c>
       <c r="J42" s="8"/>
@@ -10808,28 +10817,28 @@
       <c r="A43" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B43" s="15">
-        <v>25.864164099237879</v>
-      </c>
-      <c r="C43" s="15">
-        <v>9.0014269498946007</v>
-      </c>
-      <c r="D43" s="15">
-        <v>29.244397600129719</v>
-      </c>
-      <c r="E43" s="15">
-        <v>4.065380249716231</v>
-      </c>
-      <c r="F43" s="15">
-        <v>99.02362574995945</v>
-      </c>
-      <c r="G43" s="15">
-        <v>0.89164910004864617</v>
-      </c>
-      <c r="H43" s="15">
+      <c r="B43" s="18">
+        <v>19.94227693940185</v>
+      </c>
+      <c r="C43" s="18">
+        <v>1.422161443832956</v>
+      </c>
+      <c r="D43" s="18">
+        <v>22.878868233520631</v>
+      </c>
+      <c r="E43" s="18">
+        <v>-0.79210946908384594</v>
+      </c>
+      <c r="F43" s="18">
+        <v>99.435322226119865</v>
+      </c>
+      <c r="G43" s="18">
+        <v>0.56467777387997586</v>
+      </c>
+      <c r="H43" s="18">
         <v>0</v>
       </c>
-      <c r="I43" s="15">
+      <c r="I43" s="18">
         <v>0</v>
       </c>
       <c r="J43" s="8"/>
@@ -10841,28 +10850,28 @@
       <c r="A44" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B44" s="15">
-        <v>12.065770739563</v>
-      </c>
-      <c r="C44" s="15">
-        <v>4.2694705403268776</v>
-      </c>
-      <c r="D44" s="15">
-        <v>24.537035331729761</v>
-      </c>
-      <c r="E44" s="15">
-        <v>2.3851167698482878</v>
-      </c>
-      <c r="F44" s="15">
-        <v>99.56438262455822</v>
-      </c>
-      <c r="G44" s="15">
-        <v>0.39931592748831379</v>
-      </c>
-      <c r="H44" s="15">
-        <v>3.6301447953483071E-2</v>
-      </c>
-      <c r="I44" s="15">
+      <c r="B44" s="18">
+        <v>11.89352908148301</v>
+      </c>
+      <c r="C44" s="18">
+        <v>8.9057695083403055E-2</v>
+      </c>
+      <c r="D44" s="18">
+        <v>24.422640481198389</v>
+      </c>
+      <c r="E44" s="18">
+        <v>-1.2343481117721229</v>
+      </c>
+      <c r="F44" s="18">
+        <v>99.775886138185072</v>
+      </c>
+      <c r="G44" s="18">
+        <v>0.1867615515124342</v>
+      </c>
+      <c r="H44" s="18">
+        <v>3.7352310302486848E-2</v>
+      </c>
+      <c r="I44" s="18">
         <v>0</v>
       </c>
       <c r="J44" s="8"/>
@@ -10874,29 +10883,29 @@
       <c r="A45" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B45" s="15">
-        <v>16.239920481101759</v>
-      </c>
-      <c r="C45" s="15">
-        <v>6.1606707707202073</v>
-      </c>
-      <c r="D45" s="15">
-        <v>23.673104387159071</v>
-      </c>
-      <c r="E45" s="15">
-        <v>0.60793745030012702</v>
-      </c>
-      <c r="F45" s="15">
-        <v>98.650803923551422</v>
-      </c>
-      <c r="G45" s="15">
-        <v>1.250207301041562</v>
-      </c>
-      <c r="H45" s="15">
-        <v>9.8988775407017907E-2</v>
-      </c>
-      <c r="I45" s="15">
-        <v>0</v>
+      <c r="B45" s="18">
+        <v>14.32148199852768</v>
+      </c>
+      <c r="C45" s="18">
+        <v>1.479616139570489</v>
+      </c>
+      <c r="D45" s="18">
+        <v>23.204049224603089</v>
+      </c>
+      <c r="E45" s="18">
+        <v>0.96912108811170061</v>
+      </c>
+      <c r="F45" s="18">
+        <v>99.129402444749772</v>
+      </c>
+      <c r="G45" s="18">
+        <v>0.82328893356332067</v>
+      </c>
+      <c r="H45" s="18">
+        <v>4.7308621686181537E-2</v>
+      </c>
+      <c r="I45" s="18">
+        <v>1.774073313213767E-2</v>
       </c>
       <c r="J45" s="8"/>
       <c r="K45" s="8"/>
@@ -10907,29 +10916,29 @@
       <c r="A46" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B46" s="15">
-        <v>23.412296168591769</v>
-      </c>
-      <c r="C46" s="15">
-        <v>5.8971505894804439</v>
-      </c>
-      <c r="D46" s="15">
-        <v>25.764683118276341</v>
-      </c>
-      <c r="E46" s="15">
-        <v>-1.471860660589787</v>
-      </c>
-      <c r="F46" s="15">
-        <v>98.315260347598723</v>
-      </c>
-      <c r="G46" s="15">
-        <v>1.585089773536539</v>
-      </c>
-      <c r="H46" s="15">
-        <v>0.12761518648640241</v>
-      </c>
-      <c r="I46" s="15">
-        <v>2.9807050356394889E-3</v>
+      <c r="B46" s="18">
+        <v>15.51616555567329</v>
+      </c>
+      <c r="C46" s="18">
+        <v>4.5097040090413792E-2</v>
+      </c>
+      <c r="D46" s="18">
+        <v>33.20745361155906</v>
+      </c>
+      <c r="E46" s="18">
+        <v>5.7562279821459574</v>
+      </c>
+      <c r="F46" s="18">
+        <v>97.992304762303164</v>
+      </c>
+      <c r="G46" s="18">
+        <v>1.8979374906461579</v>
+      </c>
+      <c r="H46" s="18">
+        <v>0.1069391968430348</v>
+      </c>
+      <c r="I46" s="18">
+        <v>2.8185502073370451E-3</v>
       </c>
       <c r="J46" s="8"/>
       <c r="K46" s="8"/>
@@ -10940,28 +10949,28 @@
       <c r="A47" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B47" s="15">
-        <v>8.5</v>
-      </c>
-      <c r="C47" s="15">
-        <v>7.8</v>
-      </c>
-      <c r="D47" s="15">
-        <v>23.8</v>
-      </c>
-      <c r="E47" s="15">
-        <v>0.6</v>
-      </c>
-      <c r="F47" s="15">
-        <v>98.7</v>
-      </c>
-      <c r="G47" s="15">
-        <v>1.3</v>
-      </c>
-      <c r="H47" s="15">
-        <v>0</v>
-      </c>
-      <c r="I47" s="15">
+      <c r="B47" s="18">
+        <v>7.6736206812886687</v>
+      </c>
+      <c r="C47" s="18">
+        <v>3.726799999999999</v>
+      </c>
+      <c r="D47" s="18">
+        <v>24.6651087614304</v>
+      </c>
+      <c r="E47" s="18">
+        <v>1.0561</v>
+      </c>
+      <c r="F47" s="18">
+        <v>98.906619385341997</v>
+      </c>
+      <c r="G47" s="18">
+        <v>1.078605200945</v>
+      </c>
+      <c r="H47" s="18">
+        <v>1.4775413711E-2</v>
+      </c>
+      <c r="I47" s="18">
         <v>0</v>
       </c>
       <c r="J47" s="8"/>
@@ -10973,28 +10982,28 @@
       <c r="A48" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B48" s="15">
-        <v>17.456177606177611</v>
-      </c>
-      <c r="C48" s="15">
-        <v>11.54993564993565</v>
-      </c>
-      <c r="D48" s="15">
-        <v>27.700514800514799</v>
-      </c>
-      <c r="E48" s="15">
-        <v>0.3248391248391248</v>
-      </c>
-      <c r="F48" s="15">
-        <v>99.681274131274137</v>
-      </c>
-      <c r="G48" s="15">
-        <v>0.31872586872586872</v>
-      </c>
-      <c r="H48" s="15">
-        <v>0</v>
-      </c>
-      <c r="I48" s="15">
+      <c r="B48" s="18">
+        <v>14.69061888465513</v>
+      </c>
+      <c r="C48" s="18">
+        <v>3.5231043114543108</v>
+      </c>
+      <c r="D48" s="18">
+        <v>29.713925743156981</v>
+      </c>
+      <c r="E48" s="18">
+        <v>2.1414968468468469</v>
+      </c>
+      <c r="F48" s="18">
+        <v>99.807320090919973</v>
+      </c>
+      <c r="G48" s="18">
+        <v>0.15414392726346529</v>
+      </c>
+      <c r="H48" s="18">
+        <v>3.853598181563192E-2</v>
+      </c>
+      <c r="I48" s="18">
         <v>0</v>
       </c>
       <c r="J48" s="8"/>
@@ -11006,28 +11015,28 @@
       <c r="A49" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B49" s="15">
-        <v>14.818362321071261</v>
-      </c>
-      <c r="C49" s="15">
-        <v>7.9608780975835014</v>
-      </c>
-      <c r="D49" s="15">
-        <v>26.457041711559182</v>
-      </c>
-      <c r="E49" s="15">
-        <v>0.36874326612282599</v>
-      </c>
-      <c r="F49" s="15">
-        <v>99.437540403263043</v>
-      </c>
-      <c r="G49" s="15">
-        <v>0.55045405571802364</v>
-      </c>
-      <c r="H49" s="15">
-        <v>1.2005541018931819E-2</v>
-      </c>
-      <c r="I49" s="15">
+      <c r="B49" s="18">
+        <v>14.799316817071601</v>
+      </c>
+      <c r="C49" s="18">
+        <v>2.5975384144006131</v>
+      </c>
+      <c r="D49" s="18">
+        <v>25.39026060144764</v>
+      </c>
+      <c r="E49" s="18">
+        <v>0.1197955112983531</v>
+      </c>
+      <c r="F49" s="18">
+        <v>99.443086384403017</v>
+      </c>
+      <c r="G49" s="18">
+        <v>0.54243718450119027</v>
+      </c>
+      <c r="H49" s="18">
+        <v>1.44764310943882E-2</v>
+      </c>
+      <c r="I49" s="18">
         <v>0</v>
       </c>
       <c r="J49" s="8"/>
@@ -11039,29 +11048,29 @@
       <c r="A50" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B50" s="15">
-        <v>13.90787401574803</v>
-      </c>
-      <c r="C50" s="15">
-        <v>10.78425196850394</v>
-      </c>
-      <c r="D50" s="15">
-        <v>19.059055118110241</v>
-      </c>
-      <c r="E50" s="15">
-        <v>-0.7338582677165354</v>
-      </c>
-      <c r="F50" s="15">
-        <v>98.066929133858252</v>
-      </c>
-      <c r="G50" s="15">
-        <v>1.5228346456692909</v>
-      </c>
-      <c r="H50" s="15">
-        <v>0.4</v>
-      </c>
-      <c r="I50" s="15">
-        <v>1.023622047244094E-2</v>
+      <c r="B50" s="18">
+        <v>12.986598646276279</v>
+      </c>
+      <c r="C50" s="18">
+        <v>3.668004172811659</v>
+      </c>
+      <c r="D50" s="18">
+        <v>19.352891181115279</v>
+      </c>
+      <c r="E50" s="18">
+        <v>0.48709237442526238</v>
+      </c>
+      <c r="F50" s="18">
+        <v>98.583836784663788</v>
+      </c>
+      <c r="G50" s="18">
+        <v>1.225596379651539</v>
+      </c>
+      <c r="H50" s="18">
+        <v>0.18069436235936789</v>
+      </c>
+      <c r="I50" s="18">
+        <v>1.4235157418904489E-2</v>
       </c>
       <c r="J50" s="8"/>
       <c r="K50" s="8"/>
@@ -11072,28 +11081,28 @@
       <c r="A51" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B51" s="15">
-        <v>9.293469030474828</v>
-      </c>
-      <c r="C51" s="15">
-        <v>8.0610765950567753</v>
-      </c>
-      <c r="D51" s="15">
-        <v>17.16305998902822</v>
-      </c>
-      <c r="E51" s="15">
-        <v>0.62440781963251146</v>
-      </c>
-      <c r="F51" s="15">
-        <v>98.528581188054389</v>
-      </c>
-      <c r="G51" s="15">
-        <v>1.296952993028597</v>
-      </c>
-      <c r="H51" s="15">
-        <v>0.22877420893968639</v>
-      </c>
-      <c r="I51" s="15">
+      <c r="B51" s="18">
+        <v>8.7594407443505933</v>
+      </c>
+      <c r="C51" s="18">
+        <v>-0.37215907946615512</v>
+      </c>
+      <c r="D51" s="18">
+        <v>16.6044719089744</v>
+      </c>
+      <c r="E51" s="18">
+        <v>0.92597965918349467</v>
+      </c>
+      <c r="F51" s="18">
+        <v>98.760255228808248</v>
+      </c>
+      <c r="G51" s="18">
+        <v>0.99747928025338373</v>
+      </c>
+      <c r="H51" s="18">
+        <v>0.2422654909378234</v>
+      </c>
+      <c r="I51" s="18">
         <v>0</v>
       </c>
       <c r="J51" s="8"/>
@@ -11105,28 +11114,28 @@
       <c r="A52" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B52" s="15">
-        <v>17.015772778239651</v>
-      </c>
-      <c r="C52" s="15">
-        <v>5.2004958925773748</v>
-      </c>
-      <c r="D52" s="15">
-        <v>22.485768498788811</v>
-      </c>
-      <c r="E52" s="15">
-        <v>6.0345050626290311</v>
-      </c>
-      <c r="F52" s="15">
-        <v>97.962391086987566</v>
-      </c>
-      <c r="G52" s="15">
-        <v>1.940579917154692</v>
-      </c>
-      <c r="H52" s="15">
-        <v>9.7028995857734612E-2</v>
-      </c>
-      <c r="I52" s="15">
+      <c r="B52" s="18">
+        <v>10.8168676237062</v>
+      </c>
+      <c r="C52" s="18">
+        <v>-0.66961514013486523</v>
+      </c>
+      <c r="D52" s="18">
+        <v>19.278544196633732</v>
+      </c>
+      <c r="E52" s="18">
+        <v>0.38545703390716612</v>
+      </c>
+      <c r="F52" s="18">
+        <v>98.73872576966933</v>
+      </c>
+      <c r="G52" s="18">
+        <v>1.261274230330673</v>
+      </c>
+      <c r="H52" s="18">
+        <v>0</v>
+      </c>
+      <c r="I52" s="18">
         <v>0</v>
       </c>
       <c r="J52" s="8"/>
@@ -11138,34 +11147,44 @@
       <c r="A53" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B53" s="15">
-        <v>10.7</v>
-      </c>
-      <c r="C53" s="15">
-        <v>11.3</v>
-      </c>
-      <c r="D53" s="15">
-        <v>14.4</v>
-      </c>
-      <c r="E53" s="15">
-        <v>3.6</v>
-      </c>
-      <c r="F53" s="15">
-        <v>99</v>
-      </c>
-      <c r="G53" s="15">
-        <v>0.8</v>
-      </c>
-      <c r="H53" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="I53" s="15">
-        <v>0.2</v>
+      <c r="B53" s="18">
+        <v>-4.1000000000000014</v>
+      </c>
+      <c r="C53" s="18">
+        <v>-5.8999999999999986</v>
+      </c>
+      <c r="D53" s="18">
+        <v>3.7</v>
+      </c>
+      <c r="E53" s="18">
+        <v>-9.8000000000000007</v>
+      </c>
+      <c r="F53" s="18">
+        <v>99.7</v>
+      </c>
+      <c r="G53" s="18">
+        <v>0.3</v>
+      </c>
+      <c r="H53" s="18">
+        <v>0</v>
+      </c>
+      <c r="I53" s="18">
+        <v>0</v>
       </c>
       <c r="J53" s="8"/>
       <c r="K53" s="8"/>
       <c r="L53" s="8"/>
       <c r="M53" s="8"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B54" s="19"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="19"/>
+      <c r="F54" s="19"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="19"/>
+      <c r="I54" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -11176,11 +11195,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC61B108-7690-FA48-BD1F-70BA8E6E6932}">
   <dimension ref="A51:A100"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="51" s="10" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="52" s="10" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -11240,23 +11259,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4E922D9-587A-2248-9CA1-A6E55F67A864}">
-  <dimension ref="A2:V5"/>
+  <dimension ref="A2:X5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="X5" sqref="X5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:22" ht="20" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:24" ht="20" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
     </row>
-    <row r="4" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
         <v>43911</v>
       </c>
@@ -11320,8 +11339,14 @@
       <c r="V4" s="5">
         <v>44051</v>
       </c>
+      <c r="W4" s="5">
+        <v>44058</v>
+      </c>
+      <c r="X4" s="5">
+        <v>44065</v>
+      </c>
     </row>
-    <row r="5" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
         <v>0.42452508300000003</v>
       </c>
@@ -11384,6 +11409,12 @@
       </c>
       <c r="V5" s="6">
         <v>0.39900000000000002</v>
+      </c>
+      <c r="W5" s="2">
+        <v>0.35874357300000004</v>
+      </c>
+      <c r="X5" s="11">
+        <v>0.35906673899999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the network data
</commit_message>
<xml_diff>
--- a/next_week.xlsx
+++ b/next_week.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rboehm/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0BC670C-F0A5-F940-9F23-432EED79BAEC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{95709F4A-41DE-0941-B494-5402B3F4C80C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="3920" windowWidth="33600" windowHeight="19560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5880" yWindow="8540" windowWidth="33600" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SG Data" sheetId="1" r:id="rId1"/>
@@ -409,7 +409,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -443,6 +443,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -792,160 +795,160 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="0">
-                  <c:v>-5.8884177131164526</c:v>
+                  <c:v>1.891202561827996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-5.5236056188720477</c:v>
+                  <c:v>5.6221490973963313</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-9.4270775392146007</c:v>
+                  <c:v>5.5694200343775924</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-5.140578560446647</c:v>
+                  <c:v>-1.0688564780217209</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-5.3628758091709177</c:v>
+                  <c:v>3.0565415332731161</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-4.8797405879514368</c:v>
+                  <c:v>-0.14146414906216889</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-3.844536204161674</c:v>
+                  <c:v>3.2469963561437152</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-8.8517705319371043</c:v>
+                  <c:v>0.52027740351756346</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-8.5800774904158157</c:v>
+                  <c:v>-0.69103728170783585</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-6.8874000000000004</c:v>
+                  <c:v>0.32969999999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-1.680915928115559</c:v>
+                  <c:v>1.624206953723397</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-7.4508516730289109</c:v>
+                  <c:v>3.64346766814529</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-22.91645104242124</c:v>
+                  <c:v>1.442048290965481</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-2.838960517655579</c:v>
+                  <c:v>-4.5736265179456073E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-6.5078523283743266</c:v>
+                  <c:v>1.3787283442134419</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-7.3617879753820166</c:v>
+                  <c:v>3.5735114501620249</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-6.6802041296335872</c:v>
+                  <c:v>0.46025888021488309</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-3.2742922086857931</c:v>
+                  <c:v>0.90438769262791452</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-7.8092544365474099</c:v>
+                  <c:v>7.8354197794041367</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-3.304026867237134</c:v>
+                  <c:v>3.981895875011241</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-2.208364271879045</c:v>
+                  <c:v>2.5141907709305018</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-6.4218264648276966</c:v>
+                  <c:v>0.42209400030845678</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-7.7935601418599836</c:v>
+                  <c:v>-0.18130131535243879</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-6.4855617680187496</c:v>
+                  <c:v>2.2118555736679371</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-4.3530912257919914</c:v>
+                  <c:v>-1.4389658211050389</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-4.4864381469897943</c:v>
+                  <c:v>3.2622698244013311</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-4.118242370343161</c:v>
+                  <c:v>4.8644908189524596</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-4.3881756766971698</c:v>
+                  <c:v>-1.082249694751414</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-2.5637280284211599</c:v>
+                  <c:v>3.6403574952807332</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-4.462739823578354</c:v>
+                  <c:v>-2.3539138700493392</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-8.5335333759039642</c:v>
+                  <c:v>-7.6822063483115988E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-8.5108655801234701</c:v>
+                  <c:v>0.1080250474247272</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-6.6490781866322406</c:v>
+                  <c:v>0.61357703482835313</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-7.0067890283831584</c:v>
+                  <c:v>1.968328785287579</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-7.0014253393217407</c:v>
+                  <c:v>7.0783522303178961</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3.7073609576553008</c:v>
+                  <c:v>0.33291852578505959</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-6.4209248755268211</c:v>
+                  <c:v>7.1078230389184096</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-3.8930617677929158</c:v>
+                  <c:v>-1.464312869628714</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-5.2152303044299817</c:v>
+                  <c:v>-0.21889985783090141</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-8.7766422218355142</c:v>
+                  <c:v>1.091466477252625</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>-6.15</c:v>
+                  <c:v>-1.4</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>-7.8562799086249084</c:v>
+                  <c:v>6.6442031104093973</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>11.92047061308765</c:v>
+                  <c:v>4.6620293966902713</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>-6.650811273304881</c:v>
+                  <c:v>3.5327653566194419</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>-5.4485944694560047</c:v>
+                  <c:v>2.418830387471107</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-3.5608</c:v>
+                  <c:v>9.5500000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>-10.10587922150131</c:v>
+                  <c:v>-0.84428104102771639</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>-7.1936525642706286</c:v>
+                  <c:v>0.38168619007107452</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>-6.8068278475058044</c:v>
+                  <c:v>1.4183965657069139E-4</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>-8.3112779457748971</c:v>
+                  <c:v>2.0201020009244481</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>-4.2806564987104352</c:v>
+                  <c:v>2.5784931188513882</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>-0.71668484649861641</c:v>
+                  <c:v>5.0138909760834238</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1024,6 +1027,7 @@
         <c:axId val="221445583"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="-5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="t"/>
@@ -1446,160 +1450,160 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="0">
-                  <c:v>-1.0550750248886771</c:v>
+                  <c:v>0.34764738693991099</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.1248867767812657E-2</c:v>
+                  <c:v>1.0580090751642679</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.3023791250959209</c:v>
+                  <c:v>0.97167263027295725</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.36822844978245889</c:v>
+                  <c:v>-2.0671907229970712</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.4631399821316684</c:v>
+                  <c:v>-0.65341160494073269</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.84175888523910791</c:v>
+                  <c:v>-0.79814750230815523</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.18712771324628369</c:v>
+                  <c:v>-0.53838816846797499</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-3.254230878001553</c:v>
+                  <c:v>-0.55478820081267344</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-5.3363044765121694</c:v>
+                  <c:v>-2.7641591417138311</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-1.5086999999999999</c:v>
+                  <c:v>-0.8891</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.3722793587129899E-2</c:v>
+                  <c:v>0.3195925015074183</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-5.0499981410415611</c:v>
+                  <c:v>1.6314263448774069</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.7162407445639349</c:v>
+                  <c:v>1.0315143315634101</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.249414541091646</c:v>
+                  <c:v>-7.2106562798954582E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.2883360692627921</c:v>
+                  <c:v>0.1265036747573684</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-2.609462262177809</c:v>
+                  <c:v>1.3787787049663449</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-0.90222037180854886</c:v>
+                  <c:v>-1.4557064874810739</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.42733215396401297</c:v>
+                  <c:v>-1.438586686229439</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-1.7511669813360939</c:v>
+                  <c:v>2.519708072145554</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-1.635546161236183</c:v>
+                  <c:v>1.790743550686976</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-1.9523235603535849</c:v>
+                  <c:v>0.57157285388558832</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-0.70567937346744214</c:v>
+                  <c:v>0.52021133083084869</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-2.8531595565629768</c:v>
+                  <c:v>-1.406314795938737</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9.0343516869031082E-2</c:v>
+                  <c:v>-0.56667053450510685</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.48881429473136512</c:v>
+                  <c:v>-0.58320616589124885</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-3.7457064427076352</c:v>
+                  <c:v>-2.28505688748549</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.6628054324649939</c:v>
+                  <c:v>0.44189538864833411</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-2.371843173304744</c:v>
+                  <c:v>-0.63117126745466656</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-1.073316425537181</c:v>
+                  <c:v>0.32437525719188542</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.6031537530042479</c:v>
+                  <c:v>-0.3935461347564771</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-2.1925536275809412</c:v>
+                  <c:v>1.90388666579442</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-2.2904198324023342</c:v>
+                  <c:v>1.1146704445011439</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-1.638229450236427</c:v>
+                  <c:v>6.2948052217287775E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-1.750279239128566</c:v>
+                  <c:v>1.5350467260587359</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-5.1713402685313401</c:v>
+                  <c:v>1.664749843664511</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>7.0190803955200778</c:v>
+                  <c:v>1.1921949902327</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-0.84376354116109686</c:v>
+                  <c:v>3.4042801103821061</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-4.5528210374034213E-2</c:v>
+                  <c:v>-1.27695041083118</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-0.656053112680129</c:v>
+                  <c:v>-0.25181941309696459</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-1.1578306117307711</c:v>
+                  <c:v>-1.1118883515443529E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>-1.8</c:v>
+                  <c:v>-0.54</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>-6.099706145509618</c:v>
+                  <c:v>3.244250706506643</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>13.368193937311981</c:v>
+                  <c:v>-4.7591725622213561</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>-0.46040799232020568</c:v>
+                  <c:v>0.73547563417116057</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>-0.31159221662797099</c:v>
+                  <c:v>-1.3799661021806801E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-4.6016000000000004</c:v>
+                  <c:v>-1.7730999999999999</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>-4.5220014824021098</c:v>
+                  <c:v>0.39375808876175739</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>-3.389075425076316</c:v>
+                  <c:v>0.33930083473825662</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>-4.969698003400663</c:v>
+                  <c:v>0.61050911479938019</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>-2.0283991508866981</c:v>
+                  <c:v>0.62521829218744607</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2.1572577260017769</c:v>
+                  <c:v>3.1289158192793942</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1.5205639960893971</c:v>
+                  <c:v>2.3408503141428172</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1678,7 +1682,8 @@
         <c:axId val="221445583"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="15"/>
+          <c:max val="6"/>
+          <c:min val="-6"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="t"/>
@@ -2106,160 +2111,160 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="0">
-                  <c:v>1.0378258193241741</c:v>
+                  <c:v>1.127420469052324</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.56624522180063308</c:v>
+                  <c:v>1.652244519765147</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.20811654526534859</c:v>
+                  <c:v>3.3545790003354579E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2082446408143439</c:v>
+                  <c:v>0.86739968786611266</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.84201515731080256</c:v>
+                  <c:v>0.88204283669931349</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.9873463753556222</c:v>
+                  <c:v>2.873435528377271</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.5702487752671752</c:v>
+                  <c:v>2.3030330211957049</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.96233412423617504</c:v>
+                  <c:v>0.78208872940028695</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.33844256718123172</c:v>
+                  <c:v>0.70811322194735449</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.84582852748899995</c:v>
+                  <c:v>1.052631578947</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.84419258827662524</c:v>
+                  <c:v>0.73575714329856579</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.6226746709120633</c:v>
+                  <c:v>1.291944911196151</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.7303754266211611</c:v>
+                  <c:v>1.8688095683049899</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.35096134284148373</c:v>
+                  <c:v>0.23760858189976161</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.39179707453944101</c:v>
+                  <c:v>0.52703535056147244</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.32647446581242218</c:v>
+                  <c:v>0.58161922700175506</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.1827654344919578E-2</c:v>
+                  <c:v>1.38748818053966E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.30741450202448101</c:v>
+                  <c:v>0.2640089999092548</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.4359482899457815</c:v>
+                  <c:v>0.81411171032652974</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.90495178079533667</c:v>
+                  <c:v>0.85279604508665419</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.22455317627292939</c:v>
+                  <c:v>0.24580361874603371</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.74827182671969039</c:v>
+                  <c:v>0.77778658993405214</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.57784185751278216</c:v>
+                  <c:v>0.47586851803239788</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.44471634291769241</c:v>
+                  <c:v>0.76941740558718108</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.51973004659190614</c:v>
+                  <c:v>0.38516330571696178</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.67093187435911739</c:v>
+                  <c:v>0.84754225050329912</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.64623200938147107</c:v>
+                  <c:v>0.9164037228050862</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.9954648526077099</c:v>
+                  <c:v>2.5791855203619911</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.17660288428759871</c:v>
+                  <c:v>6.1404432476111818E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.1285440878964339</c:v>
+                  <c:v>0.94100813796099803</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.34649788587967367</c:v>
+                  <c:v>0.23771657018346321</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.85185979224978348</c:v>
+                  <c:v>0.78239268238761994</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.480670884104484</c:v>
+                  <c:v>1.1354223114624269</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1.243862922513149</c:v>
+                  <c:v>1.1487605634260729</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.54963286401610267</c:v>
+                  <c:v>1.196538544763305</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.11210202116779321</c:v>
+                  <c:v>0.1108637953841014</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.46242530457616099</c:v>
+                  <c:v>1.0132910707356571</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.2844734580533379</c:v>
+                  <c:v>0.23228904209560619</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.80260392025365845</c:v>
+                  <c:v>0.73396565647200762</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.53311326137312931</c:v>
+                  <c:v>0.52302718065649811</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.32</c:v>
+                  <c:v>0.23</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.65845197047286441</c:v>
+                  <c:v>1.007942154469196</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3.7892144888663312E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.94456597482018534</c:v>
+                  <c:v>1.3664989017566671</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.98729994527226439</c:v>
+                  <c:v>1.03861847799947</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.71070234113700004</c:v>
+                  <c:v>0.95341868700599997</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.18589630528509621</c:v>
+                  <c:v>0.18433379597501731</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.42211228372749998</c:v>
+                  <c:v>0.48797256051790161</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.001508800110017</c:v>
+                  <c:v>1.496803556525943</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1.53982654489577</c:v>
+                  <c:v>1.665076092264699</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1.0013195302767079</c:v>
+                  <c:v>1.246642181571441</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1.790073230268511</c:v>
+                  <c:v>2.2727272727272729</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2765,28 +2770,28 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="0">
-                  <c:v>7.361578758263225E-2</c:v>
+                  <c:v>0.10302222963218249</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9586551203264239E-2</c:v>
+                  <c:v>0.30219648628918733</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.20603763494182961</c:v>
+                  <c:v>0.1704071841712208</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.1981420722526325</c:v>
+                  <c:v>0.13756295604899579</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.9634807471703604E-2</c:v>
+                  <c:v>8.5238861336880495E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.3548583213341022E-2</c:v>
+                  <c:v>5.5251502120061489E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.9384985303933897E-2</c:v>
+                  <c:v>8.5073893174122339E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2795,130 +2800,130 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.17944683305176501</c:v>
+                  <c:v>0.20340260363886889</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.804376366241626E-2</c:v>
+                  <c:v>7.6090850657204043E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.7921880925293902E-2</c:v>
+                  <c:v>3.7376191366099792E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.667964808069427E-3</c:v>
+                  <c:v>1.370915931200197E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.7744116202128051E-2</c:v>
+                  <c:v>6.3241931001078722E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>1.38748818053966E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.8147175188671379E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.1008642543842192</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.19950668992344781</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="17">
-                  <c:v>3.8994906290365818E-2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.9205154415636711E-2</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.23887603179164199</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1.8445478511343431E-2</c:v>
-                </c:pt>
                 <c:pt idx="21">
-                  <c:v>6.1840646831384759E-3</c:v>
+                  <c:v>2.4623539888870911E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.1584563644624996E-2</c:v>
+                  <c:v>6.2636069680818529E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.8736869444254897E-2</c:v>
+                  <c:v>5.4891640300660668E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4.0748509990436978E-2</c:v>
+                  <c:v>2.4552801177144309E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.149733113445841</c:v>
+                  <c:v>0.11136650866057329</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>5.2661409030068169E-2</c:v>
+                  <c:v>9.1670864635351401E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.31746031746031739</c:v>
+                  <c:v>0.31674208144796379</c:v>
                 </c:pt>
                 <c:pt idx="28">
+                  <c:v>2.0691676436107861E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.1082716441354879</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7.9238856727232895E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.691212610180836E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.52826991190839145</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.1248454735785003</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.12602885705099851</c:v>
+                </c:pt>
+                <c:pt idx="35">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="29">
-                  <c:v>2.0392017704833721E-2</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>3.174152603656049E-2</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>2.512376286945588E-2</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.36133023745462178</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>9.2060045921656813E-2</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>1.8961726054164688E-2</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>5.6051010583896617E-2</c:v>
-                </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.6387391133658089E-2</c:v>
+                  <c:v>5.2173831163889073E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4.1402163133410497E-2</c:v>
+                  <c:v>2.713269475285434E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.1074838882122176</c:v>
+                  <c:v>0.1234813804593974</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1.995095437251659E-2</c:v>
+                  <c:v>2.9330299908469571E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.09</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>4.4130535410005632E-2</c:v>
+                  <c:v>7.0332908781463144E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.13602890145700919</c:v>
+                  <c:v>0.27003878238689832</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>8.6569000912372837E-2</c:v>
+                  <c:v>9.4481743498184348E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0</c:v>
+                  <c:v>1.3620266957000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0</c:v>
+                  <c:v>3.8121259837232822E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>4.5936051981044839E-3</c:v>
+                  <c:v>1.653602303417125E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.26297756884710899</c:v>
+                  <c:v>0.5385929837242831</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.1074071611641176</c:v>
+                  <c:v>0.17064174422115169</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2.8609129436477379E-2</c:v>
+                  <c:v>8.4998330561689192E-2</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>8.1366965012205042E-2</c:v>
+                  <c:v>0.32467532467532467</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3425,28 +3430,28 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="0">
-                  <c:v>9.350551071997967E-3</c:v>
+                  <c:v>1.6634539252294311E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.12392369842448089</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.948975872487228E-2</c:v>
+                  <c:v>2.5488530293653739E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.4569699473080572E-2</c:v>
+                  <c:v>2.8680570655460931E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.6145270355696508E-3</c:v>
+                  <c:v>1.639446723567747E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.0764035573348981E-3</c:v>
+                  <c:v>2.1085749952961839E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -3458,7 +3463,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.435887311675692E-2</c:v>
+                  <c:v>3.4149812504307951E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -3479,85 +3484,85 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>2.0442279371101778E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.1376071796239869E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
+                  <c:v>1.852219093608426E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="20">
-                  <c:v>1.8445478511343431E-2</c:v>
-                </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1.507043445098437E-2</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>6.8538898955539662E-3</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.8301232751170887E-2</c:v>
+                  <c:v>7.3426527768664693E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>2.3123688473789952E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.5351473922902487E-2</c:v>
+                  <c:v>9.0497737556561084E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4.7552793891437392E-2</c:v>
+                  <c:v>6.0931938572598307E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>9.1277377104923146E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.1548558160512627</c:v>
+                  <c:v>0.27671281099951439</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>5.1149859747446737E-3</c:v>
+                  <c:v>3.2738626727199182E-3</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.1602876756941151E-3</c:v>
+                  <c:v>3.1507214262749641E-3</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0</c:v>
+                  <c:v>9.8086346303512938E-3</c:v>
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>7.8028241135778839E-3</c:v>
+                  <c:v>2.332987705525107E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>9.9754771862582935E-3</c:v>
+                  <c:v>6.5922456660089529E-3</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0</c:v>
+                  <c:v>4.3958067988414458E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>4.518796994871499E-2</c:v>
+                  <c:v>0.11259164513982441</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.179979601269892E-2</c:v>
+                  <c:v>1.589646196979929E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>0</c:v>
@@ -3569,16 +3574,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0</c:v>
+                  <c:v>1.328039932554336E-2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0</c:v>
+                  <c:v>4.2660436055287923E-2</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>7.1522823591193439E-3</c:v>
+                  <c:v>7.0831942134740979E-3</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>8.1366965012205042E-2</c:v>
+                  <c:v>8.1168831168831168E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4080,160 +4085,160 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="0">
-                  <c:v>28.491100844211729</c:v>
+                  <c:v>28.93669107437249</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29.0038958675275</c:v>
+                  <c:v>32.195069420957111</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>47.279305354558623</c:v>
+                  <c:v>47.76663249963822</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.970790192941031</c:v>
+                  <c:v>29.60107929662675</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30.24222096761363</c:v>
+                  <c:v>30.424383566574399</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>34.917965566202078</c:v>
+                  <c:v>32.50269786011529</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20.972897425097901</c:v>
+                  <c:v>25.392362152896851</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>34.401834353897939</c:v>
+                  <c:v>33.513899447549107</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>22.159409474280409</c:v>
+                  <c:v>19.83074085726297</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16.205587460016901</c:v>
+                  <c:v>15.3245752490444</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>27.160927177874711</c:v>
+                  <c:v>24.03888026926515</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>24.214138455361489</c:v>
+                  <c:v>29.294805964711141</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>39.924643779668088</c:v>
+                  <c:v>37.381987523472482</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.0644812131283921</c:v>
+                  <c:v>2.0290704281227789</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>24.31577014798307</c:v>
+                  <c:v>23.39549779704209</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>22.896832478601869</c:v>
+                  <c:v>26.914222157788089</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.6389802108350051</c:v>
+                  <c:v>0.54252234733844151</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>24.106057825035158</c:v>
+                  <c:v>22.040821977771341</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>24.514564353457189</c:v>
+                  <c:v>35.548606866686818</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>37.24176413859476</c:v>
+                  <c:v>39.265941752227917</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>35.740081963070011</c:v>
+                  <c:v>35.562437666912153</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>27.74053872292691</c:v>
+                  <c:v>25.26424603633669</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>30.920750970236309</c:v>
+                  <c:v>28.60728279501992</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>31.777989645767541</c:v>
+                  <c:v>35.147296546242707</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>29.90568336623998</c:v>
+                  <c:v>26.426261915417779</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>26.57021436877293</c:v>
+                  <c:v>27.25572856671694</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>21.645157545954561</c:v>
+                  <c:v>25.373020620814948</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>29.068873017530411</c:v>
+                  <c:v>29.735200667511069</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>23.14753607731069</c:v>
+                  <c:v>19.542682783481709</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>29.500789032007749</c:v>
+                  <c:v>27.479632442878451</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>33.146706527813372</c:v>
+                  <c:v>30.841923466947311</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>19.736133298441992</c:v>
+                  <c:v>16.697989367927001</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>38.774716696450639</c:v>
+                  <c:v>37.817886729074708</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>27.780448696406388</c:v>
+                  <c:v>28.348656506749659</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>33.687007512858827</c:v>
+                  <c:v>40.340639349059998</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>16.709564607523919</c:v>
+                  <c:v>16.200745004709169</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>29.36764113980982</c:v>
+                  <c:v>39.337571211507807</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>24.122665095773851</c:v>
+                  <c:v>21.516596309967628</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>31.069534194055141</c:v>
+                  <c:v>29.13244171131711</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>24.456926741065001</c:v>
+                  <c:v>24.277028319372171</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>32.04</c:v>
+                  <c:v>30.83</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>33.942424617239332</c:v>
+                  <c:v>41.760357247987358</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>12.745934515718179</c:v>
+                  <c:v>12.60859439596986</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>29.60139398309801</c:v>
+                  <c:v>32.998274021308887</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>31.13721906391498</c:v>
+                  <c:v>31.096253709325371</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>23.369988341752499</c:v>
+                  <c:v>24.398644741866601</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>34.028674668803852</c:v>
+                  <c:v>33.420778277803713</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>24.111482119563629</c:v>
+                  <c:v>23.962424638410639</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>25.1656795271258</c:v>
+                  <c:v>23.885385422716791</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>32.741645368305051</c:v>
+                  <c:v>33.514670687587802</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>25.152893713609021</c:v>
+                  <c:v>30.27595154980045</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>25.38791053193734</c:v>
+                  <c:v>26.01792308327509</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4734,160 +4739,160 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="0">
-                  <c:v>49.379482004771603</c:v>
+                  <c:v>51.087144616748972</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45.463949909725663</c:v>
+                  <c:v>47.897631871363537</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>63.414634146341477</c:v>
+                  <c:v>56.706998985879324</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>52.072177606855817</c:v>
+                  <c:v>48.864821004198838</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38.64517591280319</c:v>
+                  <c:v>38.016803804804823</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>61.906390905477153</c:v>
+                  <c:v>60.877855614341229</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43.770886577651858</c:v>
+                  <c:v>40.102710261559501</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>60.510217334743757</c:v>
+                  <c:v>59.879470777623411</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44.180639447469296</c:v>
+                  <c:v>42.035916265420809</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>50.377499999999998</c:v>
+                  <c:v>48.676900000000003</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45.323178873895827</c:v>
+                  <c:v>43.18489681951057</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43.370936243213777</c:v>
+                  <c:v>51.108582403529283</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>62.370066296579331</c:v>
+                  <c:v>59.778036840393128</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>52.59074777836986</c:v>
+                  <c:v>48.154729385985249</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>46.910358720090947</c:v>
+                  <c:v>46.259310526006317</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>37.970697812523639</c:v>
+                  <c:v>41.826236679611007</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>37.642220197427903</c:v>
+                  <c:v>34.722772470075419</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>42.304347685621757</c:v>
+                  <c:v>42.949658544331562</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>39.45416442745956</c:v>
+                  <c:v>47.214468724029459</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>45.356527608121162</c:v>
+                  <c:v>50.256359745039227</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>64.982904511484904</c:v>
+                  <c:v>66.035848382348647</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>48.175636288845332</c:v>
+                  <c:v>46.258901989926542</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>58.758377298464517</c:v>
+                  <c:v>54.887127066458632</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>48.76578147298725</c:v>
+                  <c:v>51.698413441099291</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>53.968022132199387</c:v>
+                  <c:v>53.706146138484897</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>32.808846633253822</c:v>
+                  <c:v>31.746395955759599</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>48.537349908346933</c:v>
+                  <c:v>49.758023797559098</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>51.203038096365148</c:v>
+                  <c:v>52.739500106767508</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>39.154021611081554</c:v>
+                  <c:v>39.270619241260583</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>54.279316992082151</c:v>
+                  <c:v>54.389610023209137</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>58.343259641259408</c:v>
+                  <c:v>55.113304221235772</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>42.54460091230618</c:v>
+                  <c:v>46.393307803982921</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>61.195784192820057</c:v>
+                  <c:v>60.523072378621023</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>46.621150789450837</c:v>
+                  <c:v>54.897844270645173</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>47.598772701578611</c:v>
+                  <c:v>57.684687518216833</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>9.8193715326581259</c:v>
+                  <c:v>9.7177170659420309</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>48.357605650551143</c:v>
+                  <c:v>56.013585024050187</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>37.715574967002738</c:v>
+                  <c:v>39.806766266447042</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>62.8421135137744</c:v>
+                  <c:v>59.786674809389147</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>46.529626611932699</c:v>
+                  <c:v>44.084556762522269</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>50.77</c:v>
+                  <c:v>50.260000000000012</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>46.892617608355039</c:v>
+                  <c:v>57.352618594529552</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>-6.8786642309971704</c:v>
+                  <c:v>-8.3425685580579589</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>45.14462534538697</c:v>
+                  <c:v>45.386641453166902</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>49.750319386849426</c:v>
+                  <c:v>52.979827829432963</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>36.811100000000003</c:v>
+                  <c:v>39.016500000000001</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>56.801709202473113</c:v>
+                  <c:v>54.025509554150553</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>44.415942815840957</c:v>
+                  <c:v>47.629952486752487</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>55.397747106706518</c:v>
+                  <c:v>59.479569590384372</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>38.672589401635094</c:v>
+                  <c:v>38.317595478031841</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>51.08676700141902</c:v>
+                  <c:v>56.615996846926663</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>42.58994215390566</c:v>
+                  <c:v>45.961616181774517</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9445,20 +9450,20 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J28" sqref="J28"/>
+      <selection pane="topRight" activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.1640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="40.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="39.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="35" style="1" customWidth="1"/>
-    <col min="7" max="7" width="36.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="34.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="39.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="41" style="1" customWidth="1"/>
+    <col min="3" max="3" width="42" style="1" customWidth="1"/>
+    <col min="4" max="4" width="42.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="41" style="1" customWidth="1"/>
+    <col min="6" max="6" width="39.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="40.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="35.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="40" style="1" customWidth="1"/>
     <col min="10" max="13" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9466,62 +9471,62 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
     </row>
     <row r="2" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="19">
-        <v>28.491100844211729</v>
-      </c>
-      <c r="C2" s="19">
-        <v>-5.8884177131164526</v>
-      </c>
-      <c r="D2" s="19">
-        <v>49.379482004771603</v>
-      </c>
-      <c r="E2" s="19">
-        <v>-1.0550750248886771</v>
-      </c>
-      <c r="F2" s="19">
-        <v>98.882387139307411</v>
-      </c>
-      <c r="G2" s="19">
-        <v>1.0378258193241741</v>
-      </c>
-      <c r="H2" s="19">
-        <v>7.361578758263225E-2</v>
-      </c>
-      <c r="I2" s="19">
-        <v>9.350551071997967E-3</v>
+      <c r="B2" s="20">
+        <v>28.93669107437249</v>
+      </c>
+      <c r="C2" s="20">
+        <v>1.891202561827996</v>
+      </c>
+      <c r="D2" s="20">
+        <v>51.087144616748972</v>
+      </c>
+      <c r="E2" s="20">
+        <v>0.34764738693991099</v>
+      </c>
+      <c r="F2" s="20">
+        <v>98.758147055209079</v>
+      </c>
+      <c r="G2" s="20">
+        <v>1.127420469052324</v>
+      </c>
+      <c r="H2" s="20">
+        <v>0.10302222963218249</v>
+      </c>
+      <c r="I2" s="20">
+        <v>1.6634539252294311E-2</v>
       </c>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
@@ -9532,29 +9537,29 @@
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="20">
-        <v>29.0038958675275</v>
-      </c>
-      <c r="C3" s="20">
-        <v>-5.5236056188720477</v>
-      </c>
-      <c r="D3" s="20">
-        <v>45.463949909725663</v>
-      </c>
-      <c r="E3" s="20">
-        <v>5.1248867767812657E-2</v>
-      </c>
-      <c r="F3" s="20">
-        <v>99.414168226995585</v>
-      </c>
-      <c r="G3" s="20">
-        <v>0.56624522180063308</v>
-      </c>
-      <c r="H3" s="20">
-        <v>1.9586551203264239E-2</v>
-      </c>
-      <c r="I3" s="20">
-        <v>0</v>
+      <c r="B3" s="21">
+        <v>32.195069420957111</v>
+      </c>
+      <c r="C3" s="21">
+        <v>5.6221490973963313</v>
+      </c>
+      <c r="D3" s="21">
+        <v>47.897631871363537</v>
+      </c>
+      <c r="E3" s="21">
+        <v>1.0580090751642679</v>
+      </c>
+      <c r="F3" s="21">
+        <v>97.951845269168871</v>
+      </c>
+      <c r="G3" s="21">
+        <v>1.652244519765147</v>
+      </c>
+      <c r="H3" s="21">
+        <v>0.30219648628918733</v>
+      </c>
+      <c r="I3" s="21">
+        <v>0.12392369842448089</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -9565,28 +9570,28 @@
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="20">
-        <v>47.279305354558623</v>
-      </c>
-      <c r="C4" s="20">
-        <v>-9.4270775392146007</v>
-      </c>
-      <c r="D4" s="20">
-        <v>63.414634146341477</v>
-      </c>
-      <c r="E4" s="20">
-        <v>-2.3023791250959209</v>
-      </c>
-      <c r="F4" s="20">
-        <v>99.791883454734659</v>
-      </c>
-      <c r="G4" s="20">
-        <v>0.20811654526534859</v>
-      </c>
-      <c r="H4" s="20">
+      <c r="B4" s="21">
+        <v>47.76663249963822</v>
+      </c>
+      <c r="C4" s="21">
+        <v>5.5694200343775924</v>
+      </c>
+      <c r="D4" s="21">
+        <v>56.706998985879324</v>
+      </c>
+      <c r="E4" s="21">
+        <v>0.97167263027295725</v>
+      </c>
+      <c r="F4" s="21">
+        <v>99.966454209996641</v>
+      </c>
+      <c r="G4" s="21">
+        <v>3.3545790003354579E-2</v>
+      </c>
+      <c r="H4" s="21">
         <v>0</v>
       </c>
-      <c r="I4" s="20">
+      <c r="I4" s="21">
         <v>0</v>
       </c>
       <c r="J4" s="4"/>
@@ -9598,29 +9603,29 @@
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="20">
-        <v>30.970790192941031</v>
-      </c>
-      <c r="C5" s="20">
-        <v>-5.140578560446647</v>
-      </c>
-      <c r="D5" s="20">
-        <v>52.072177606855817</v>
-      </c>
-      <c r="E5" s="20">
-        <v>-0.36822844978245889</v>
-      </c>
-      <c r="F5" s="20">
-        <v>98.572180987858317</v>
-      </c>
-      <c r="G5" s="20">
-        <v>1.2082446408143439</v>
-      </c>
-      <c r="H5" s="20">
-        <v>0.20603763494182961</v>
-      </c>
-      <c r="I5" s="20">
-        <v>1.948975872487228E-2</v>
+      <c r="B5" s="21">
+        <v>29.60107929662675</v>
+      </c>
+      <c r="C5" s="21">
+        <v>-1.0688564780217209</v>
+      </c>
+      <c r="D5" s="21">
+        <v>48.864821004198838</v>
+      </c>
+      <c r="E5" s="21">
+        <v>-2.0671907229970712</v>
+      </c>
+      <c r="F5" s="21">
+        <v>98.942609924688696</v>
+      </c>
+      <c r="G5" s="21">
+        <v>0.86739968786611266</v>
+      </c>
+      <c r="H5" s="21">
+        <v>0.1704071841712208</v>
+      </c>
+      <c r="I5" s="21">
+        <v>2.5488530293653739E-2</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
@@ -9631,28 +9636,28 @@
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="20">
-        <v>30.24222096761363</v>
-      </c>
-      <c r="C6" s="20">
-        <v>-5.3628758091709177</v>
-      </c>
-      <c r="D6" s="20">
-        <v>38.64517591280319</v>
-      </c>
-      <c r="E6" s="20">
-        <v>-0.4631399821316684</v>
-      </c>
-      <c r="F6" s="20">
-        <v>98.959842770435998</v>
-      </c>
-      <c r="G6" s="20">
-        <v>0.84201515731080256</v>
-      </c>
-      <c r="H6" s="20">
-        <v>0.1981420722526325</v>
-      </c>
-      <c r="I6" s="20">
+      <c r="B6" s="21">
+        <v>30.424383566574399</v>
+      </c>
+      <c r="C6" s="21">
+        <v>3.0565415332731161</v>
+      </c>
+      <c r="D6" s="21">
+        <v>38.016803804804823</v>
+      </c>
+      <c r="E6" s="21">
+        <v>-0.65341160494073269</v>
+      </c>
+      <c r="F6" s="21">
+        <v>98.980394207251379</v>
+      </c>
+      <c r="G6" s="21">
+        <v>0.88204283669931349</v>
+      </c>
+      <c r="H6" s="21">
+        <v>0.13756295604899579</v>
+      </c>
+      <c r="I6" s="21">
         <v>0</v>
       </c>
       <c r="J6" s="4"/>
@@ -9664,29 +9669,29 @@
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="20">
-        <v>34.917965566202078</v>
-      </c>
-      <c r="C7" s="20">
-        <v>-4.8797405879514368</v>
-      </c>
-      <c r="D7" s="20">
-        <v>61.906390905477153</v>
-      </c>
-      <c r="E7" s="20">
-        <v>0.84175888523910791</v>
-      </c>
-      <c r="F7" s="20">
-        <v>96.898449117698789</v>
-      </c>
-      <c r="G7" s="20">
-        <v>2.9873463753556222</v>
-      </c>
-      <c r="H7" s="20">
-        <v>8.9634807471703604E-2</v>
-      </c>
-      <c r="I7" s="20">
-        <v>2.4569699473080572E-2</v>
+      <c r="B7" s="21">
+        <v>32.50269786011529</v>
+      </c>
+      <c r="C7" s="21">
+        <v>-0.14146414906216889</v>
+      </c>
+      <c r="D7" s="21">
+        <v>60.877855614341229</v>
+      </c>
+      <c r="E7" s="21">
+        <v>-0.79814750230815523</v>
+      </c>
+      <c r="F7" s="21">
+        <v>97.012645039629987</v>
+      </c>
+      <c r="G7" s="21">
+        <v>2.873435528377271</v>
+      </c>
+      <c r="H7" s="21">
+        <v>8.5238861336880495E-2</v>
+      </c>
+      <c r="I7" s="21">
+        <v>2.8680570655460931E-2</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -9697,29 +9702,29 @@
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="20">
-        <v>20.972897425097901</v>
-      </c>
-      <c r="C8" s="20">
-        <v>-3.844536204161674</v>
-      </c>
-      <c r="D8" s="20">
-        <v>43.770886577651858</v>
-      </c>
-      <c r="E8" s="20">
-        <v>0.18712771324628369</v>
-      </c>
-      <c r="F8" s="20">
-        <v>97.370588114482985</v>
-      </c>
-      <c r="G8" s="20">
-        <v>2.5702487752671752</v>
-      </c>
-      <c r="H8" s="20">
-        <v>5.3548583213341022E-2</v>
-      </c>
-      <c r="I8" s="20">
-        <v>5.6145270355696508E-3</v>
+      <c r="B8" s="21">
+        <v>25.392362152896851</v>
+      </c>
+      <c r="C8" s="21">
+        <v>3.2469963561437152</v>
+      </c>
+      <c r="D8" s="21">
+        <v>40.102710261559501</v>
+      </c>
+      <c r="E8" s="21">
+        <v>-0.53838816846797499</v>
+      </c>
+      <c r="F8" s="21">
+        <v>97.625321009446708</v>
+      </c>
+      <c r="G8" s="21">
+        <v>2.3030330211957049</v>
+      </c>
+      <c r="H8" s="21">
+        <v>5.5251502120061489E-2</v>
+      </c>
+      <c r="I8" s="21">
+        <v>1.639446723567747E-2</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
@@ -9730,29 +9735,29 @@
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="20">
-        <v>34.401834353897939</v>
-      </c>
-      <c r="C9" s="20">
-        <v>-8.8517705319371043</v>
-      </c>
-      <c r="D9" s="20">
-        <v>60.510217334743757</v>
-      </c>
-      <c r="E9" s="20">
-        <v>-3.254230878001553</v>
-      </c>
-      <c r="F9" s="20">
-        <v>98.958280890459278</v>
-      </c>
-      <c r="G9" s="20">
-        <v>0.96233412423617504</v>
-      </c>
-      <c r="H9" s="20">
-        <v>7.9384985303933897E-2</v>
-      </c>
-      <c r="I9" s="20">
-        <v>7.0764035573348981E-3</v>
+      <c r="B9" s="21">
+        <v>33.513899447549107</v>
+      </c>
+      <c r="C9" s="21">
+        <v>0.52027740351756346</v>
+      </c>
+      <c r="D9" s="21">
+        <v>59.879470777623411</v>
+      </c>
+      <c r="E9" s="21">
+        <v>-0.55478820081267344</v>
+      </c>
+      <c r="F9" s="21">
+        <v>99.132837377424991</v>
+      </c>
+      <c r="G9" s="21">
+        <v>0.78208872940028695</v>
+      </c>
+      <c r="H9" s="21">
+        <v>8.5073893174122339E-2</v>
+      </c>
+      <c r="I9" s="21">
+        <v>2.1085749952961839E-2</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -9763,28 +9768,28 @@
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="20">
-        <v>22.159409474280409</v>
-      </c>
-      <c r="C10" s="20">
-        <v>-8.5800774904158157</v>
-      </c>
-      <c r="D10" s="20">
-        <v>44.180639447469296</v>
-      </c>
-      <c r="E10" s="20">
-        <v>-5.3363044765121694</v>
-      </c>
-      <c r="F10" s="20">
-        <v>99.661557432817887</v>
-      </c>
-      <c r="G10" s="20">
-        <v>0.33844256718123172</v>
-      </c>
-      <c r="H10" s="20">
+      <c r="B10" s="21">
+        <v>19.83074085726297</v>
+      </c>
+      <c r="C10" s="21">
+        <v>-0.69103728170783585</v>
+      </c>
+      <c r="D10" s="21">
+        <v>42.035916265420809</v>
+      </c>
+      <c r="E10" s="21">
+        <v>-2.7641591417138311</v>
+      </c>
+      <c r="F10" s="21">
+        <v>99.291886778051776</v>
+      </c>
+      <c r="G10" s="21">
+        <v>0.70811322194735449</v>
+      </c>
+      <c r="H10" s="21">
         <v>0</v>
       </c>
-      <c r="I10" s="20">
+      <c r="I10" s="21">
         <v>0</v>
       </c>
       <c r="J10" s="4"/>
@@ -9796,28 +9801,28 @@
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="20">
-        <v>16.205587460016901</v>
-      </c>
-      <c r="C11" s="20">
-        <v>-6.8874000000000004</v>
-      </c>
-      <c r="D11" s="20">
-        <v>50.377499999999998</v>
-      </c>
-      <c r="E11" s="20">
-        <v>-1.5086999999999999</v>
-      </c>
-      <c r="F11" s="20">
-        <v>99.154171472510001</v>
-      </c>
-      <c r="G11" s="20">
-        <v>0.84582852748899995</v>
-      </c>
-      <c r="H11" s="20">
+      <c r="B11" s="21">
+        <v>15.3245752490444</v>
+      </c>
+      <c r="C11" s="21">
+        <v>0.32969999999999999</v>
+      </c>
+      <c r="D11" s="21">
+        <v>48.676900000000003</v>
+      </c>
+      <c r="E11" s="21">
+        <v>-0.8891</v>
+      </c>
+      <c r="F11" s="21">
+        <v>98.947368421052005</v>
+      </c>
+      <c r="G11" s="21">
+        <v>1.052631578947</v>
+      </c>
+      <c r="H11" s="21">
         <v>0</v>
       </c>
-      <c r="I11" s="20">
+      <c r="I11" s="21">
         <v>0</v>
       </c>
       <c r="J11" s="4"/>
@@ -9829,28 +9834,28 @@
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="20">
-        <v>27.160927177874711</v>
-      </c>
-      <c r="C12" s="20">
-        <v>-1.680915928115559</v>
-      </c>
-      <c r="D12" s="20">
-        <v>45.323178873895827</v>
-      </c>
-      <c r="E12" s="20">
-        <v>9.3722793587129899E-2</v>
-      </c>
-      <c r="F12" s="20">
-        <v>98.976360578670395</v>
-      </c>
-      <c r="G12" s="20">
-        <v>0.84419258827662524</v>
-      </c>
-      <c r="H12" s="20">
-        <v>0.17944683305176501</v>
-      </c>
-      <c r="I12" s="20">
+      <c r="B12" s="21">
+        <v>24.03888026926515</v>
+      </c>
+      <c r="C12" s="21">
+        <v>1.624206953723397</v>
+      </c>
+      <c r="D12" s="21">
+        <v>43.18489681951057</v>
+      </c>
+      <c r="E12" s="21">
+        <v>0.3195925015074183</v>
+      </c>
+      <c r="F12" s="21">
+        <v>99.060840253061357</v>
+      </c>
+      <c r="G12" s="21">
+        <v>0.73575714329856579</v>
+      </c>
+      <c r="H12" s="21">
+        <v>0.20340260363886889</v>
+      </c>
+      <c r="I12" s="21">
         <v>0</v>
       </c>
       <c r="J12" s="4"/>
@@ -9862,29 +9867,29 @@
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="20">
-        <v>24.214138455361489</v>
-      </c>
-      <c r="C13" s="20">
-        <v>-7.4508516730289109</v>
-      </c>
-      <c r="D13" s="20">
-        <v>43.370936243213777</v>
-      </c>
-      <c r="E13" s="20">
-        <v>-5.0499981410415611</v>
-      </c>
-      <c r="F13" s="20">
-        <v>99.345901947222018</v>
-      </c>
-      <c r="G13" s="20">
-        <v>0.6226746709120633</v>
-      </c>
-      <c r="H13" s="20">
-        <v>2.804376366241626E-2</v>
-      </c>
-      <c r="I13" s="20">
-        <v>1.435887311675692E-2</v>
+      <c r="B13" s="21">
+        <v>29.294805964711141</v>
+      </c>
+      <c r="C13" s="21">
+        <v>3.64346766814529</v>
+      </c>
+      <c r="D13" s="21">
+        <v>51.108582403529283</v>
+      </c>
+      <c r="E13" s="21">
+        <v>1.6314263448774069</v>
+      </c>
+      <c r="F13" s="21">
+        <v>98.605071616207397</v>
+      </c>
+      <c r="G13" s="21">
+        <v>1.291944911196151</v>
+      </c>
+      <c r="H13" s="21">
+        <v>7.6090850657204043E-2</v>
+      </c>
+      <c r="I13" s="21">
+        <v>3.4149812504307951E-2</v>
       </c>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
@@ -9895,28 +9900,28 @@
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="20">
-        <v>39.924643779668088</v>
-      </c>
-      <c r="C14" s="20">
-        <v>-22.91645104242124</v>
-      </c>
-      <c r="D14" s="20">
-        <v>62.370066296579331</v>
-      </c>
-      <c r="E14" s="20">
-        <v>1.7162407445639349</v>
-      </c>
-      <c r="F14" s="20">
-        <v>97.231702692453553</v>
-      </c>
-      <c r="G14" s="20">
-        <v>2.7303754266211611</v>
-      </c>
-      <c r="H14" s="20">
-        <v>3.7921880925293902E-2</v>
-      </c>
-      <c r="I14" s="20">
+      <c r="B14" s="21">
+        <v>37.381987523472482</v>
+      </c>
+      <c r="C14" s="21">
+        <v>1.442048290965481</v>
+      </c>
+      <c r="D14" s="21">
+        <v>59.778036840393128</v>
+      </c>
+      <c r="E14" s="21">
+        <v>1.0315143315634101</v>
+      </c>
+      <c r="F14" s="21">
+        <v>98.093814240328911</v>
+      </c>
+      <c r="G14" s="21">
+        <v>1.8688095683049899</v>
+      </c>
+      <c r="H14" s="21">
+        <v>3.7376191366099792E-2</v>
+      </c>
+      <c r="I14" s="21">
         <v>0</v>
       </c>
       <c r="J14" s="4"/>
@@ -9928,28 +9933,28 @@
       <c r="A15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="20">
-        <v>6.0644812131283921</v>
-      </c>
-      <c r="C15" s="20">
-        <v>-2.838960517655579</v>
-      </c>
-      <c r="D15" s="20">
-        <v>52.59074777836986</v>
-      </c>
-      <c r="E15" s="20">
-        <v>1.249414541091646</v>
-      </c>
-      <c r="F15" s="20">
-        <v>99.649038657158513</v>
-      </c>
-      <c r="G15" s="20">
-        <v>0.35096134284148373</v>
-      </c>
-      <c r="H15" s="20">
+      <c r="B15" s="21">
+        <v>2.0290704281227789</v>
+      </c>
+      <c r="C15" s="21">
+        <v>-4.5736265179456073E-2</v>
+      </c>
+      <c r="D15" s="21">
+        <v>48.154729385985249</v>
+      </c>
+      <c r="E15" s="21">
+        <v>-7.2106562798954582E-2</v>
+      </c>
+      <c r="F15" s="21">
+        <v>99.762391418100222</v>
+      </c>
+      <c r="G15" s="21">
+        <v>0.23760858189976161</v>
+      </c>
+      <c r="H15" s="21">
         <v>0</v>
       </c>
-      <c r="I15" s="20">
+      <c r="I15" s="21">
         <v>0</v>
       </c>
       <c r="J15" s="4"/>
@@ -9961,28 +9966,28 @@
       <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="20">
-        <v>24.31577014798307</v>
-      </c>
-      <c r="C16" s="20">
-        <v>-6.5078523283743266</v>
-      </c>
-      <c r="D16" s="20">
-        <v>46.910358720090947</v>
-      </c>
-      <c r="E16" s="20">
-        <v>1.2883360692627921</v>
-      </c>
-      <c r="F16" s="20">
-        <v>99.605534960651639</v>
-      </c>
-      <c r="G16" s="20">
-        <v>0.39179707453944101</v>
-      </c>
-      <c r="H16" s="20">
-        <v>2.667964808069427E-3</v>
-      </c>
-      <c r="I16" s="20">
+      <c r="B16" s="21">
+        <v>23.39549779704209</v>
+      </c>
+      <c r="C16" s="21">
+        <v>1.3787283442134419</v>
+      </c>
+      <c r="D16" s="21">
+        <v>46.259310526006317</v>
+      </c>
+      <c r="E16" s="21">
+        <v>0.1265036747573684</v>
+      </c>
+      <c r="F16" s="21">
+        <v>99.459255490124804</v>
+      </c>
+      <c r="G16" s="21">
+        <v>0.52703535056147244</v>
+      </c>
+      <c r="H16" s="21">
+        <v>1.370915931200197E-2</v>
+      </c>
+      <c r="I16" s="21">
         <v>0</v>
       </c>
       <c r="J16" s="4"/>
@@ -9994,28 +9999,28 @@
       <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="20">
-        <v>22.896832478601869</v>
-      </c>
-      <c r="C17" s="20">
-        <v>-7.3617879753820166</v>
-      </c>
-      <c r="D17" s="20">
-        <v>37.970697812523639</v>
-      </c>
-      <c r="E17" s="20">
-        <v>-2.609462262177809</v>
-      </c>
-      <c r="F17" s="20">
-        <v>99.655781417983988</v>
-      </c>
-      <c r="G17" s="20">
-        <v>0.32647446581242218</v>
-      </c>
-      <c r="H17" s="20">
-        <v>1.7744116202128051E-2</v>
-      </c>
-      <c r="I17" s="20">
+      <c r="B17" s="21">
+        <v>26.914222157788089</v>
+      </c>
+      <c r="C17" s="21">
+        <v>3.5735114501620249</v>
+      </c>
+      <c r="D17" s="21">
+        <v>41.826236679611007</v>
+      </c>
+      <c r="E17" s="21">
+        <v>1.3787787049663449</v>
+      </c>
+      <c r="F17" s="21">
+        <v>99.355138841996421</v>
+      </c>
+      <c r="G17" s="21">
+        <v>0.58161922700175506</v>
+      </c>
+      <c r="H17" s="21">
+        <v>6.3241931001078722E-2</v>
+      </c>
+      <c r="I17" s="21">
         <v>0</v>
       </c>
       <c r="J17" s="4"/>
@@ -10027,28 +10032,28 @@
       <c r="A18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="20">
-        <v>2.6389802108350051</v>
-      </c>
-      <c r="C18" s="20">
-        <v>-6.6802041296335872</v>
-      </c>
-      <c r="D18" s="20">
-        <v>37.642220197427903</v>
-      </c>
-      <c r="E18" s="20">
-        <v>-0.90222037180854886</v>
-      </c>
-      <c r="F18" s="20">
-        <v>99.958172345655086</v>
-      </c>
-      <c r="G18" s="20">
-        <v>4.1827654344919578E-2</v>
-      </c>
-      <c r="H18" s="20">
-        <v>0</v>
-      </c>
-      <c r="I18" s="20">
+      <c r="B18" s="21">
+        <v>0.54252234733844151</v>
+      </c>
+      <c r="C18" s="21">
+        <v>0.46025888021488309</v>
+      </c>
+      <c r="D18" s="21">
+        <v>34.722772470075419</v>
+      </c>
+      <c r="E18" s="21">
+        <v>-1.4557064874810739</v>
+      </c>
+      <c r="F18" s="21">
+        <v>99.9722502363892</v>
+      </c>
+      <c r="G18" s="21">
+        <v>1.38748818053966E-2</v>
+      </c>
+      <c r="H18" s="21">
+        <v>1.38748818053966E-2</v>
+      </c>
+      <c r="I18" s="21">
         <v>0</v>
       </c>
       <c r="J18" s="4"/>
@@ -10060,28 +10065,28 @@
       <c r="A19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="20">
-        <v>24.106057825035158</v>
-      </c>
-      <c r="C19" s="20">
-        <v>-3.2742922086857931</v>
-      </c>
-      <c r="D19" s="20">
-        <v>42.304347685621757</v>
-      </c>
-      <c r="E19" s="20">
-        <v>0.42733215396401297</v>
-      </c>
-      <c r="F19" s="20">
-        <v>99.653590591685159</v>
-      </c>
-      <c r="G19" s="20">
-        <v>0.30741450202448101</v>
-      </c>
-      <c r="H19" s="20">
-        <v>3.8994906290365818E-2</v>
-      </c>
-      <c r="I19" s="20">
+      <c r="B19" s="21">
+        <v>22.040821977771341</v>
+      </c>
+      <c r="C19" s="21">
+        <v>0.90438769262791452</v>
+      </c>
+      <c r="D19" s="21">
+        <v>42.949658544331562</v>
+      </c>
+      <c r="E19" s="21">
+        <v>-1.438586686229439</v>
+      </c>
+      <c r="F19" s="21">
+        <v>99.677843824902027</v>
+      </c>
+      <c r="G19" s="21">
+        <v>0.2640089999092548</v>
+      </c>
+      <c r="H19" s="21">
+        <v>5.8147175188671379E-2</v>
+      </c>
+      <c r="I19" s="21">
         <v>0</v>
       </c>
       <c r="J19" s="4"/>
@@ -10093,29 +10098,29 @@
       <c r="A20" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="20">
-        <v>24.514564353457189</v>
-      </c>
-      <c r="C20" s="20">
-        <v>-7.8092544365474099</v>
-      </c>
-      <c r="D20" s="20">
-        <v>39.45416442745956</v>
-      </c>
-      <c r="E20" s="20">
-        <v>-1.7511669813360939</v>
-      </c>
-      <c r="F20" s="20">
-        <v>99.5448465556385</v>
-      </c>
-      <c r="G20" s="20">
-        <v>0.4359482899457815</v>
-      </c>
-      <c r="H20" s="20">
-        <v>1.9205154415636711E-2</v>
-      </c>
-      <c r="I20" s="20">
-        <v>0</v>
+      <c r="B20" s="21">
+        <v>35.548606866686818</v>
+      </c>
+      <c r="C20" s="21">
+        <v>7.8354197794041367</v>
+      </c>
+      <c r="D20" s="21">
+        <v>47.214468724029459</v>
+      </c>
+      <c r="E20" s="21">
+        <v>2.519708072145554</v>
+      </c>
+      <c r="F20" s="21">
+        <v>99.064581755918056</v>
+      </c>
+      <c r="G20" s="21">
+        <v>0.81411171032652974</v>
+      </c>
+      <c r="H20" s="21">
+        <v>0.1008642543842192</v>
+      </c>
+      <c r="I20" s="21">
+        <v>2.0442279371101778E-2</v>
       </c>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
@@ -10126,29 +10131,29 @@
       <c r="A21" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="20">
-        <v>37.24176413859476</v>
-      </c>
-      <c r="C21" s="20">
-        <v>-3.304026867237134</v>
-      </c>
-      <c r="D21" s="20">
-        <v>45.356527608121162</v>
-      </c>
-      <c r="E21" s="20">
-        <v>-1.635546161236183</v>
-      </c>
-      <c r="F21" s="20">
-        <v>98.856172187412739</v>
-      </c>
-      <c r="G21" s="20">
-        <v>0.90495178079533667</v>
-      </c>
-      <c r="H21" s="20">
-        <v>0.23887603179164199</v>
-      </c>
-      <c r="I21" s="20">
-        <v>0</v>
+      <c r="B21" s="21">
+        <v>39.265941752227917</v>
+      </c>
+      <c r="C21" s="21">
+        <v>3.981895875011241</v>
+      </c>
+      <c r="D21" s="21">
+        <v>50.256359745039227</v>
+      </c>
+      <c r="E21" s="21">
+        <v>1.790743550686976</v>
+      </c>
+      <c r="F21" s="21">
+        <v>98.92632119319353</v>
+      </c>
+      <c r="G21" s="21">
+        <v>0.85279604508665419</v>
+      </c>
+      <c r="H21" s="21">
+        <v>0.19950668992344781</v>
+      </c>
+      <c r="I21" s="21">
+        <v>2.1376071796239869E-2</v>
       </c>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
@@ -10159,29 +10164,29 @@
       <c r="A22" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="20">
-        <v>35.740081963070011</v>
-      </c>
-      <c r="C22" s="20">
-        <v>-2.208364271879045</v>
-      </c>
-      <c r="D22" s="20">
-        <v>64.982904511484904</v>
-      </c>
-      <c r="E22" s="20">
-        <v>-1.9523235603535849</v>
-      </c>
-      <c r="F22" s="20">
-        <v>99.738555866704317</v>
-      </c>
-      <c r="G22" s="20">
-        <v>0.22455317627292939</v>
-      </c>
-      <c r="H22" s="20">
-        <v>1.8445478511343431E-2</v>
-      </c>
-      <c r="I22" s="20">
-        <v>1.8445478511343431E-2</v>
+      <c r="B22" s="21">
+        <v>35.562437666912153</v>
+      </c>
+      <c r="C22" s="21">
+        <v>2.5141907709305018</v>
+      </c>
+      <c r="D22" s="21">
+        <v>66.035848382348647</v>
+      </c>
+      <c r="E22" s="21">
+        <v>0.57157285388558832</v>
+      </c>
+      <c r="F22" s="21">
+        <v>99.754196381253891</v>
+      </c>
+      <c r="G22" s="21">
+        <v>0.24580361874603371</v>
+      </c>
+      <c r="H22" s="21">
+        <v>0</v>
+      </c>
+      <c r="I22" s="21">
+        <v>0</v>
       </c>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
@@ -10192,29 +10197,29 @@
       <c r="A23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="20">
-        <v>27.74053872292691</v>
-      </c>
-      <c r="C23" s="20">
-        <v>-6.4218264648276966</v>
-      </c>
-      <c r="D23" s="20">
-        <v>48.175636288845332</v>
-      </c>
-      <c r="E23" s="20">
-        <v>-0.70567937346744214</v>
-      </c>
-      <c r="F23" s="20">
-        <v>99.245544108595169</v>
-      </c>
-      <c r="G23" s="20">
-        <v>0.74827182671969039</v>
-      </c>
-      <c r="H23" s="20">
-        <v>6.1840646831384759E-3</v>
-      </c>
-      <c r="I23" s="20">
-        <v>0</v>
+      <c r="B23" s="21">
+        <v>25.26424603633669</v>
+      </c>
+      <c r="C23" s="21">
+        <v>0.42209400030845678</v>
+      </c>
+      <c r="D23" s="21">
+        <v>46.258901989926542</v>
+      </c>
+      <c r="E23" s="21">
+        <v>0.52021133083084869</v>
+      </c>
+      <c r="F23" s="21">
+        <v>99.197589870176088</v>
+      </c>
+      <c r="G23" s="21">
+        <v>0.77778658993405214</v>
+      </c>
+      <c r="H23" s="21">
+        <v>2.4623539888870911E-2</v>
+      </c>
+      <c r="I23" s="21">
+        <v>1.852219093608426E-2</v>
       </c>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
@@ -10225,29 +10230,29 @@
       <c r="A24" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="20">
-        <v>30.920750970236309</v>
-      </c>
-      <c r="C24" s="20">
-        <v>-7.7935601418599836</v>
-      </c>
-      <c r="D24" s="20">
-        <v>58.758377298464517</v>
-      </c>
-      <c r="E24" s="20">
-        <v>-2.8531595565629768</v>
-      </c>
-      <c r="F24" s="20">
-        <v>99.35057357884169</v>
-      </c>
-      <c r="G24" s="20">
-        <v>0.57784185751278216</v>
-      </c>
-      <c r="H24" s="20">
-        <v>7.1584563644624996E-2</v>
-      </c>
-      <c r="I24" s="20">
-        <v>1.507043445098437E-2</v>
+      <c r="B24" s="21">
+        <v>28.60728279501992</v>
+      </c>
+      <c r="C24" s="21">
+        <v>-0.18130131535243879</v>
+      </c>
+      <c r="D24" s="21">
+        <v>54.887127066458632</v>
+      </c>
+      <c r="E24" s="21">
+        <v>-1.406314795938737</v>
+      </c>
+      <c r="F24" s="21">
+        <v>99.461495412285018</v>
+      </c>
+      <c r="G24" s="21">
+        <v>0.47586851803239788</v>
+      </c>
+      <c r="H24" s="21">
+        <v>6.2636069680818529E-2</v>
+      </c>
+      <c r="I24" s="21">
+        <v>0</v>
       </c>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
@@ -10258,29 +10263,29 @@
       <c r="A25" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="20">
-        <v>31.777989645767541</v>
-      </c>
-      <c r="C25" s="20">
-        <v>-6.4855617680187496</v>
-      </c>
-      <c r="D25" s="20">
-        <v>48.76578147298725</v>
-      </c>
-      <c r="E25" s="20">
-        <v>9.0343516869031082E-2</v>
-      </c>
-      <c r="F25" s="20">
-        <v>99.509692897741132</v>
-      </c>
-      <c r="G25" s="20">
-        <v>0.44471634291769241</v>
-      </c>
-      <c r="H25" s="20">
-        <v>3.8736869444254897E-2</v>
-      </c>
-      <c r="I25" s="20">
-        <v>6.8538898955539662E-3</v>
+      <c r="B25" s="21">
+        <v>35.147296546242707</v>
+      </c>
+      <c r="C25" s="21">
+        <v>2.2118555736679371</v>
+      </c>
+      <c r="D25" s="21">
+        <v>51.698413441099291</v>
+      </c>
+      <c r="E25" s="21">
+        <v>-0.56667053450510685</v>
+      </c>
+      <c r="F25" s="21">
+        <v>99.175690954110777</v>
+      </c>
+      <c r="G25" s="21">
+        <v>0.76941740558718108</v>
+      </c>
+      <c r="H25" s="21">
+        <v>5.4891640300660668E-2</v>
+      </c>
+      <c r="I25" s="21">
+        <v>0</v>
       </c>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
@@ -10291,28 +10296,28 @@
       <c r="A26" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="20">
-        <v>29.90568336623998</v>
-      </c>
-      <c r="C26" s="20">
-        <v>-4.3530912257919914</v>
-      </c>
-      <c r="D26" s="20">
-        <v>53.968022132199387</v>
-      </c>
-      <c r="E26" s="20">
-        <v>0.48881429473136512</v>
-      </c>
-      <c r="F26" s="20">
-        <v>99.439521443416993</v>
-      </c>
-      <c r="G26" s="20">
-        <v>0.51973004659190614</v>
-      </c>
-      <c r="H26" s="20">
-        <v>4.0748509990436978E-2</v>
-      </c>
-      <c r="I26" s="20">
+      <c r="B26" s="21">
+        <v>26.426261915417779</v>
+      </c>
+      <c r="C26" s="21">
+        <v>-1.4389658211050389</v>
+      </c>
+      <c r="D26" s="21">
+        <v>53.706146138484897</v>
+      </c>
+      <c r="E26" s="21">
+        <v>-0.58320616589124885</v>
+      </c>
+      <c r="F26" s="21">
+        <v>99.590283893105209</v>
+      </c>
+      <c r="G26" s="21">
+        <v>0.38516330571696178</v>
+      </c>
+      <c r="H26" s="21">
+        <v>2.4552801177144309E-2</v>
+      </c>
+      <c r="I26" s="21">
         <v>0</v>
       </c>
       <c r="J26" s="4"/>
@@ -10324,29 +10329,29 @@
       <c r="A27" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="20">
-        <v>26.57021436877293</v>
-      </c>
-      <c r="C27" s="20">
-        <v>-4.4864381469897943</v>
-      </c>
-      <c r="D27" s="20">
-        <v>32.808846633253822</v>
-      </c>
-      <c r="E27" s="20">
-        <v>-3.7457064427076352</v>
-      </c>
-      <c r="F27" s="20">
-        <v>99.159610100417652</v>
-      </c>
-      <c r="G27" s="20">
-        <v>0.67093187435911739</v>
-      </c>
-      <c r="H27" s="20">
-        <v>0.149733113445841</v>
-      </c>
-      <c r="I27" s="20">
-        <v>3.8301232751170887E-2</v>
+      <c r="B27" s="21">
+        <v>27.25572856671694</v>
+      </c>
+      <c r="C27" s="21">
+        <v>3.2622698244013311</v>
+      </c>
+      <c r="D27" s="21">
+        <v>31.746395955759599</v>
+      </c>
+      <c r="E27" s="21">
+        <v>-2.28505688748549</v>
+      </c>
+      <c r="F27" s="21">
+        <v>99.041091240835172</v>
+      </c>
+      <c r="G27" s="21">
+        <v>0.84754225050329912</v>
+      </c>
+      <c r="H27" s="21">
+        <v>0.11136650866057329</v>
+      </c>
+      <c r="I27" s="21">
+        <v>7.3426527768664693E-2</v>
       </c>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
@@ -10357,29 +10362,29 @@
       <c r="A28" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="20">
-        <v>21.645157545954561</v>
-      </c>
-      <c r="C28" s="20">
-        <v>-4.118242370343161</v>
-      </c>
-      <c r="D28" s="20">
-        <v>48.537349908346933</v>
-      </c>
-      <c r="E28" s="20">
-        <v>1.6628054324649939</v>
-      </c>
-      <c r="F28" s="20">
-        <v>99.3011065815884</v>
-      </c>
-      <c r="G28" s="20">
-        <v>0.64623200938147107</v>
-      </c>
-      <c r="H28" s="20">
-        <v>5.2661409030068169E-2</v>
-      </c>
-      <c r="I28" s="20">
-        <v>0</v>
+      <c r="B28" s="21">
+        <v>25.373020620814948</v>
+      </c>
+      <c r="C28" s="21">
+        <v>4.8644908189524596</v>
+      </c>
+      <c r="D28" s="21">
+        <v>49.758023797559098</v>
+      </c>
+      <c r="E28" s="21">
+        <v>0.44189538864833411</v>
+      </c>
+      <c r="F28" s="21">
+        <v>98.968801724085679</v>
+      </c>
+      <c r="G28" s="21">
+        <v>0.9164037228050862</v>
+      </c>
+      <c r="H28" s="21">
+        <v>9.1670864635351401E-2</v>
+      </c>
+      <c r="I28" s="21">
+        <v>2.3123688473789952E-2</v>
       </c>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
@@ -10390,29 +10395,29 @@
       <c r="A29" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="20">
-        <v>29.068873017530411</v>
-      </c>
-      <c r="C29" s="20">
-        <v>-4.3881756766971698</v>
-      </c>
-      <c r="D29" s="20">
-        <v>51.203038096365148</v>
-      </c>
-      <c r="E29" s="20">
-        <v>-2.371843173304744</v>
-      </c>
-      <c r="F29" s="20">
-        <v>97.641723356009066</v>
-      </c>
-      <c r="G29" s="20">
-        <v>1.9954648526077099</v>
-      </c>
-      <c r="H29" s="20">
-        <v>0.31746031746031739</v>
-      </c>
-      <c r="I29" s="20">
-        <v>4.5351473922902487E-2</v>
+      <c r="B29" s="21">
+        <v>29.735200667511069</v>
+      </c>
+      <c r="C29" s="21">
+        <v>-1.082249694751414</v>
+      </c>
+      <c r="D29" s="21">
+        <v>52.739500106767508</v>
+      </c>
+      <c r="E29" s="21">
+        <v>-0.63117126745466656</v>
+      </c>
+      <c r="F29" s="21">
+        <v>97.013574660633481</v>
+      </c>
+      <c r="G29" s="21">
+        <v>2.5791855203619911</v>
+      </c>
+      <c r="H29" s="21">
+        <v>0.31674208144796379</v>
+      </c>
+      <c r="I29" s="21">
+        <v>9.0497737556561084E-2</v>
       </c>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
@@ -10423,28 +10428,28 @@
       <c r="A30" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="20">
-        <v>23.14753607731069</v>
-      </c>
-      <c r="C30" s="20">
-        <v>-2.5637280284211599</v>
-      </c>
-      <c r="D30" s="20">
-        <v>39.154021611081554</v>
-      </c>
-      <c r="E30" s="20">
-        <v>-1.073316425537181</v>
-      </c>
-      <c r="F30" s="20">
-        <v>99.823397115712396</v>
-      </c>
-      <c r="G30" s="20">
-        <v>0.17660288428759871</v>
-      </c>
-      <c r="H30" s="20">
-        <v>0</v>
-      </c>
-      <c r="I30" s="20">
+      <c r="B30" s="21">
+        <v>19.542682783481709</v>
+      </c>
+      <c r="C30" s="21">
+        <v>3.6403574952807332</v>
+      </c>
+      <c r="D30" s="21">
+        <v>39.270619241260583</v>
+      </c>
+      <c r="E30" s="21">
+        <v>0.32437525719188542</v>
+      </c>
+      <c r="F30" s="21">
+        <v>99.922042226374998</v>
+      </c>
+      <c r="G30" s="21">
+        <v>6.1404432476111818E-2</v>
+      </c>
+      <c r="H30" s="21">
+        <v>2.0691676436107861E-2</v>
+      </c>
+      <c r="I30" s="21">
         <v>0</v>
       </c>
       <c r="J30" s="4"/>
@@ -10456,29 +10461,29 @@
       <c r="A31" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="20">
-        <v>29.500789032007749</v>
-      </c>
-      <c r="C31" s="20">
-        <v>-4.462739823578354</v>
-      </c>
-      <c r="D31" s="20">
-        <v>54.279316992082151</v>
-      </c>
-      <c r="E31" s="20">
-        <v>1.6031537530042479</v>
-      </c>
-      <c r="F31" s="20">
-        <v>98.796699470895774</v>
-      </c>
-      <c r="G31" s="20">
-        <v>1.1285440878964339</v>
-      </c>
-      <c r="H31" s="20">
-        <v>2.0392017704833721E-2</v>
-      </c>
-      <c r="I31" s="20">
-        <v>4.7552793891437392E-2</v>
+      <c r="B31" s="21">
+        <v>27.479632442878451</v>
+      </c>
+      <c r="C31" s="21">
+        <v>-2.3539138700493392</v>
+      </c>
+      <c r="D31" s="21">
+        <v>54.389610023209137</v>
+      </c>
+      <c r="E31" s="21">
+        <v>-0.3935461347564771</v>
+      </c>
+      <c r="F31" s="21">
+        <v>98.889788279330915</v>
+      </c>
+      <c r="G31" s="21">
+        <v>0.94100813796099803</v>
+      </c>
+      <c r="H31" s="21">
+        <v>0.1082716441354879</v>
+      </c>
+      <c r="I31" s="21">
+        <v>6.0931938572598307E-2</v>
       </c>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
@@ -10489,28 +10494,28 @@
       <c r="A32" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="20">
-        <v>33.146706527813372</v>
-      </c>
-      <c r="C32" s="20">
-        <v>-8.5335333759039642</v>
-      </c>
-      <c r="D32" s="20">
-        <v>58.343259641259408</v>
-      </c>
-      <c r="E32" s="20">
-        <v>-2.1925536275809412</v>
-      </c>
-      <c r="F32" s="20">
-        <v>99.621760588081997</v>
-      </c>
-      <c r="G32" s="20">
-        <v>0.34649788587967367</v>
-      </c>
-      <c r="H32" s="20">
-        <v>3.174152603656049E-2</v>
-      </c>
-      <c r="I32" s="20">
+      <c r="B32" s="21">
+        <v>30.841923466947311</v>
+      </c>
+      <c r="C32" s="21">
+        <v>-7.6822063483115988E-2</v>
+      </c>
+      <c r="D32" s="21">
+        <v>55.113304221235772</v>
+      </c>
+      <c r="E32" s="21">
+        <v>1.90388666579442</v>
+      </c>
+      <c r="F32" s="21">
+        <v>99.683044573087528</v>
+      </c>
+      <c r="G32" s="21">
+        <v>0.23771657018346321</v>
+      </c>
+      <c r="H32" s="21">
+        <v>7.9238856727232895E-2</v>
+      </c>
+      <c r="I32" s="21">
         <v>0</v>
       </c>
       <c r="J32" s="4"/>
@@ -10522,29 +10527,29 @@
       <c r="A33" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B33" s="20">
-        <v>19.736133298441992</v>
-      </c>
-      <c r="C33" s="20">
-        <v>-8.5108655801234701</v>
-      </c>
-      <c r="D33" s="20">
-        <v>42.54460091230618</v>
-      </c>
-      <c r="E33" s="20">
-        <v>-2.2904198324023342</v>
-      </c>
-      <c r="F33" s="20">
-        <v>99.11388870716911</v>
-      </c>
-      <c r="G33" s="20">
-        <v>0.85185979224978348</v>
-      </c>
-      <c r="H33" s="20">
-        <v>2.512376286945588E-2</v>
-      </c>
-      <c r="I33" s="20">
-        <v>9.1277377104923146E-3</v>
+      <c r="B33" s="21">
+        <v>16.697989367927001</v>
+      </c>
+      <c r="C33" s="21">
+        <v>0.1080250474247272</v>
+      </c>
+      <c r="D33" s="21">
+        <v>46.393307803982921</v>
+      </c>
+      <c r="E33" s="21">
+        <v>1.1146704445011439</v>
+      </c>
+      <c r="F33" s="21">
+        <v>99.200695191509993</v>
+      </c>
+      <c r="G33" s="21">
+        <v>0.78239268238761994</v>
+      </c>
+      <c r="H33" s="21">
+        <v>1.691212610180836E-2</v>
+      </c>
+      <c r="I33" s="21">
+        <v>0</v>
       </c>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
@@ -10555,29 +10560,29 @@
       <c r="A34" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B34" s="20">
-        <v>38.774716696450639</v>
-      </c>
-      <c r="C34" s="20">
-        <v>-6.6490781866322406</v>
-      </c>
-      <c r="D34" s="20">
-        <v>61.195784192820057</v>
-      </c>
-      <c r="E34" s="20">
-        <v>-1.638229450236427</v>
-      </c>
-      <c r="F34" s="20">
-        <v>98.157998878439201</v>
-      </c>
-      <c r="G34" s="20">
-        <v>1.480670884104484</v>
-      </c>
-      <c r="H34" s="20">
-        <v>0.36133023745462178</v>
-      </c>
-      <c r="I34" s="20">
-        <v>0.1548558160512627</v>
+      <c r="B34" s="21">
+        <v>37.817886729074708</v>
+      </c>
+      <c r="C34" s="21">
+        <v>0.61357703482835313</v>
+      </c>
+      <c r="D34" s="21">
+        <v>60.523072378621023</v>
+      </c>
+      <c r="E34" s="21">
+        <v>6.2948052217287775E-2</v>
+      </c>
+      <c r="F34" s="21">
+        <v>98.33630777662836</v>
+      </c>
+      <c r="G34" s="21">
+        <v>1.1354223114624269</v>
+      </c>
+      <c r="H34" s="21">
+        <v>0.52826991190839145</v>
+      </c>
+      <c r="I34" s="21">
+        <v>0.27671281099951439</v>
       </c>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
@@ -10588,29 +10593,29 @@
       <c r="A35" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B35" s="20">
-        <v>27.780448696406388</v>
-      </c>
-      <c r="C35" s="20">
-        <v>-7.0067890283831584</v>
-      </c>
-      <c r="D35" s="20">
-        <v>46.621150789450837</v>
-      </c>
-      <c r="E35" s="20">
-        <v>-1.750279239128566</v>
-      </c>
-      <c r="F35" s="20">
-        <v>98.658962045590442</v>
-      </c>
-      <c r="G35" s="20">
-        <v>1.243862922513149</v>
-      </c>
-      <c r="H35" s="20">
-        <v>9.2060045921656813E-2</v>
-      </c>
-      <c r="I35" s="20">
-        <v>5.1149859747446737E-3</v>
+      <c r="B35" s="21">
+        <v>28.348656506749659</v>
+      </c>
+      <c r="C35" s="21">
+        <v>1.968328785287579</v>
+      </c>
+      <c r="D35" s="21">
+        <v>54.897844270645173</v>
+      </c>
+      <c r="E35" s="21">
+        <v>1.5350467260587359</v>
+      </c>
+      <c r="F35" s="21">
+        <v>98.723120100322717</v>
+      </c>
+      <c r="G35" s="21">
+        <v>1.1487605634260729</v>
+      </c>
+      <c r="H35" s="21">
+        <v>0.1248454735785003</v>
+      </c>
+      <c r="I35" s="21">
+        <v>3.2738626727199182E-3</v>
       </c>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
@@ -10621,29 +10626,29 @@
       <c r="A36" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B36" s="20">
-        <v>33.687007512858827</v>
-      </c>
-      <c r="C36" s="20">
-        <v>-7.0014253393217407</v>
-      </c>
-      <c r="D36" s="20">
-        <v>47.598772701578611</v>
-      </c>
-      <c r="E36" s="20">
-        <v>-5.1713402685313401</v>
-      </c>
-      <c r="F36" s="20">
-        <v>99.428245122254026</v>
-      </c>
-      <c r="G36" s="20">
-        <v>0.54963286401610267</v>
-      </c>
-      <c r="H36" s="20">
-        <v>1.8961726054164688E-2</v>
-      </c>
-      <c r="I36" s="20">
-        <v>3.1602876756941151E-3</v>
+      <c r="B36" s="21">
+        <v>40.340639349059998</v>
+      </c>
+      <c r="C36" s="21">
+        <v>7.0783522303178961</v>
+      </c>
+      <c r="D36" s="21">
+        <v>57.684687518216833</v>
+      </c>
+      <c r="E36" s="21">
+        <v>1.664749843664511</v>
+      </c>
+      <c r="F36" s="21">
+        <v>98.674281876759423</v>
+      </c>
+      <c r="G36" s="21">
+        <v>1.196538544763305</v>
+      </c>
+      <c r="H36" s="21">
+        <v>0.12602885705099851</v>
+      </c>
+      <c r="I36" s="21">
+        <v>3.1507214262749641E-3</v>
       </c>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
@@ -10654,28 +10659,28 @@
       <c r="A37" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B37" s="20">
-        <v>16.709564607523919</v>
-      </c>
-      <c r="C37" s="20">
-        <v>3.7073609576553008</v>
-      </c>
-      <c r="D37" s="20">
-        <v>9.8193715326581259</v>
-      </c>
-      <c r="E37" s="20">
-        <v>7.0190803955200778</v>
-      </c>
-      <c r="F37" s="20">
-        <v>99.8318469682483</v>
-      </c>
-      <c r="G37" s="20">
-        <v>0.11210202116779321</v>
-      </c>
-      <c r="H37" s="20">
-        <v>5.6051010583896617E-2</v>
-      </c>
-      <c r="I37" s="20">
+      <c r="B37" s="21">
+        <v>16.200745004709169</v>
+      </c>
+      <c r="C37" s="21">
+        <v>0.33291852578505959</v>
+      </c>
+      <c r="D37" s="21">
+        <v>9.7177170659420309</v>
+      </c>
+      <c r="E37" s="21">
+        <v>1.1921949902327</v>
+      </c>
+      <c r="F37" s="21">
+        <v>99.889136204615895</v>
+      </c>
+      <c r="G37" s="21">
+        <v>0.1108637953841014</v>
+      </c>
+      <c r="H37" s="21">
+        <v>0</v>
+      </c>
+      <c r="I37" s="21">
         <v>0</v>
       </c>
       <c r="J37" s="4"/>
@@ -10687,29 +10692,29 @@
       <c r="A38" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B38" s="20">
-        <v>29.36764113980982</v>
-      </c>
-      <c r="C38" s="20">
-        <v>-6.4209248755268211</v>
-      </c>
-      <c r="D38" s="20">
-        <v>48.357605650551143</v>
-      </c>
-      <c r="E38" s="20">
-        <v>-0.84376354116109686</v>
-      </c>
-      <c r="F38" s="20">
-        <v>99.521187304290152</v>
-      </c>
-      <c r="G38" s="20">
-        <v>0.46242530457616099</v>
-      </c>
-      <c r="H38" s="20">
-        <v>1.6387391133658089E-2</v>
-      </c>
-      <c r="I38" s="20">
-        <v>0</v>
+      <c r="B38" s="21">
+        <v>39.337571211507807</v>
+      </c>
+      <c r="C38" s="21">
+        <v>7.1078230389184096</v>
+      </c>
+      <c r="D38" s="21">
+        <v>56.013585024050187</v>
+      </c>
+      <c r="E38" s="21">
+        <v>3.4042801103821061</v>
+      </c>
+      <c r="F38" s="21">
+        <v>98.92472646347008</v>
+      </c>
+      <c r="G38" s="21">
+        <v>1.0132910707356571</v>
+      </c>
+      <c r="H38" s="21">
+        <v>5.2173831163889073E-2</v>
+      </c>
+      <c r="I38" s="21">
+        <v>9.8086346303512938E-3</v>
       </c>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
@@ -10720,28 +10725,28 @@
       <c r="A39" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B39" s="20">
-        <v>24.122665095773851</v>
-      </c>
-      <c r="C39" s="20">
-        <v>-3.8930617677929158</v>
-      </c>
-      <c r="D39" s="20">
-        <v>37.715574967002738</v>
-      </c>
-      <c r="E39" s="20">
-        <v>-4.5528210374034213E-2</v>
-      </c>
-      <c r="F39" s="20">
-        <v>99.674124378813261</v>
-      </c>
-      <c r="G39" s="20">
-        <v>0.2844734580533379</v>
-      </c>
-      <c r="H39" s="20">
-        <v>4.1402163133410497E-2</v>
-      </c>
-      <c r="I39" s="20">
+      <c r="B39" s="21">
+        <v>21.516596309967628</v>
+      </c>
+      <c r="C39" s="21">
+        <v>-1.464312869628714</v>
+      </c>
+      <c r="D39" s="21">
+        <v>39.806766266447042</v>
+      </c>
+      <c r="E39" s="21">
+        <v>-1.27695041083118</v>
+      </c>
+      <c r="F39" s="21">
+        <v>99.740578263151534</v>
+      </c>
+      <c r="G39" s="21">
+        <v>0.23228904209560619</v>
+      </c>
+      <c r="H39" s="21">
+        <v>2.713269475285434E-2</v>
+      </c>
+      <c r="I39" s="21">
         <v>0</v>
       </c>
       <c r="J39" s="4"/>
@@ -10753,29 +10758,29 @@
       <c r="A40" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B40" s="20">
-        <v>31.069534194055141</v>
-      </c>
-      <c r="C40" s="20">
-        <v>-5.2152303044299817</v>
-      </c>
-      <c r="D40" s="20">
-        <v>62.8421135137744</v>
-      </c>
-      <c r="E40" s="20">
-        <v>-0.656053112680129</v>
-      </c>
-      <c r="F40" s="20">
-        <v>99.082109367419747</v>
-      </c>
-      <c r="G40" s="20">
-        <v>0.80260392025365845</v>
-      </c>
-      <c r="H40" s="20">
-        <v>0.1074838882122176</v>
-      </c>
-      <c r="I40" s="20">
-        <v>7.8028241135778839E-3</v>
+      <c r="B40" s="21">
+        <v>29.13244171131711</v>
+      </c>
+      <c r="C40" s="21">
+        <v>-0.21889985783090141</v>
+      </c>
+      <c r="D40" s="21">
+        <v>59.786674809389147</v>
+      </c>
+      <c r="E40" s="21">
+        <v>-0.25181941309696459</v>
+      </c>
+      <c r="F40" s="21">
+        <v>99.119223086012539</v>
+      </c>
+      <c r="G40" s="21">
+        <v>0.73396565647200762</v>
+      </c>
+      <c r="H40" s="21">
+        <v>0.1234813804593974</v>
+      </c>
+      <c r="I40" s="21">
+        <v>2.332987705525107E-2</v>
       </c>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
@@ -10786,29 +10791,29 @@
       <c r="A41" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B41" s="20">
-        <v>24.456926741065001</v>
-      </c>
-      <c r="C41" s="20">
-        <v>-8.7766422218355142</v>
-      </c>
-      <c r="D41" s="20">
-        <v>46.529626611932699</v>
-      </c>
-      <c r="E41" s="20">
-        <v>-1.1578306117307711</v>
-      </c>
-      <c r="F41" s="20">
-        <v>99.446935784253398</v>
-      </c>
-      <c r="G41" s="20">
-        <v>0.53311326137312931</v>
-      </c>
-      <c r="H41" s="20">
-        <v>1.995095437251659E-2</v>
-      </c>
-      <c r="I41" s="20">
-        <v>9.9754771862582935E-3</v>
+      <c r="B41" s="21">
+        <v>24.277028319372171</v>
+      </c>
+      <c r="C41" s="21">
+        <v>1.091466477252625</v>
+      </c>
+      <c r="D41" s="21">
+        <v>44.084556762522269</v>
+      </c>
+      <c r="E41" s="21">
+        <v>-1.1118883515443529E-2</v>
+      </c>
+      <c r="F41" s="21">
+        <v>99.447642519434069</v>
+      </c>
+      <c r="G41" s="21">
+        <v>0.52302718065649811</v>
+      </c>
+      <c r="H41" s="21">
+        <v>2.9330299908469571E-2</v>
+      </c>
+      <c r="I41" s="21">
+        <v>6.5922456660089529E-3</v>
       </c>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
@@ -10819,28 +10824,28 @@
       <c r="A42" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B42" s="20">
-        <v>32.04</v>
-      </c>
-      <c r="C42" s="20">
-        <v>-6.15</v>
-      </c>
-      <c r="D42" s="20">
-        <v>50.77</v>
-      </c>
-      <c r="E42" s="20">
-        <v>-1.8</v>
-      </c>
-      <c r="F42" s="20">
-        <v>99.59</v>
-      </c>
-      <c r="G42" s="20">
-        <v>0.32</v>
-      </c>
-      <c r="H42" s="20">
-        <v>0.09</v>
-      </c>
-      <c r="I42" s="20">
+      <c r="B42" s="21">
+        <v>30.83</v>
+      </c>
+      <c r="C42" s="21">
+        <v>-1.4</v>
+      </c>
+      <c r="D42" s="21">
+        <v>50.260000000000012</v>
+      </c>
+      <c r="E42" s="21">
+        <v>-0.54</v>
+      </c>
+      <c r="F42" s="21">
+        <v>99.77000000000001</v>
+      </c>
+      <c r="G42" s="21">
+        <v>0.23</v>
+      </c>
+      <c r="H42" s="21">
+        <v>0</v>
+      </c>
+      <c r="I42" s="21">
         <v>0</v>
       </c>
       <c r="J42" s="4"/>
@@ -10852,29 +10857,29 @@
       <c r="A43" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B43" s="20">
-        <v>33.942424617239332</v>
-      </c>
-      <c r="C43" s="20">
-        <v>-7.8562799086249084</v>
-      </c>
-      <c r="D43" s="20">
-        <v>46.892617608355039</v>
-      </c>
-      <c r="E43" s="20">
-        <v>-6.099706145509618</v>
-      </c>
-      <c r="F43" s="20">
-        <v>99.297417494116971</v>
-      </c>
-      <c r="G43" s="20">
-        <v>0.65845197047286441</v>
-      </c>
-      <c r="H43" s="20">
-        <v>4.4130535410005632E-2</v>
-      </c>
-      <c r="I43" s="20">
-        <v>0</v>
+      <c r="B43" s="21">
+        <v>41.760357247987358</v>
+      </c>
+      <c r="C43" s="21">
+        <v>6.6442031104093973</v>
+      </c>
+      <c r="D43" s="21">
+        <v>57.352618594529552</v>
+      </c>
+      <c r="E43" s="21">
+        <v>3.244250706506643</v>
+      </c>
+      <c r="F43" s="21">
+        <v>98.877766868760759</v>
+      </c>
+      <c r="G43" s="21">
+        <v>1.007942154469196</v>
+      </c>
+      <c r="H43" s="21">
+        <v>7.0332908781463144E-2</v>
+      </c>
+      <c r="I43" s="21">
+        <v>4.3958067988414458E-2</v>
       </c>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
@@ -10885,28 +10890,28 @@
       <c r="A44" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B44" s="20">
-        <v>12.745934515718179</v>
-      </c>
-      <c r="C44" s="20">
-        <v>11.92047061308765</v>
-      </c>
-      <c r="D44" s="20">
-        <v>-6.8786642309971704</v>
-      </c>
-      <c r="E44" s="20">
-        <v>13.368193937311981</v>
-      </c>
-      <c r="F44" s="20">
-        <v>99.962107855111327</v>
-      </c>
-      <c r="G44" s="20">
-        <v>3.7892144888663312E-2</v>
-      </c>
-      <c r="H44" s="20">
+      <c r="B44" s="21">
+        <v>12.60859439596986</v>
+      </c>
+      <c r="C44" s="21">
+        <v>4.6620293966902713</v>
+      </c>
+      <c r="D44" s="21">
+        <v>-8.3425685580579589</v>
+      </c>
+      <c r="E44" s="21">
+        <v>-4.7591725622213561</v>
+      </c>
+      <c r="F44" s="21">
+        <v>99.999999999999986</v>
+      </c>
+      <c r="G44" s="21">
         <v>0</v>
       </c>
-      <c r="I44" s="20">
+      <c r="H44" s="21">
+        <v>0</v>
+      </c>
+      <c r="I44" s="21">
         <v>0</v>
       </c>
       <c r="J44" s="4"/>
@@ -10918,29 +10923,29 @@
       <c r="A45" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B45" s="20">
-        <v>29.60139398309801</v>
-      </c>
-      <c r="C45" s="20">
-        <v>-6.650811273304881</v>
-      </c>
-      <c r="D45" s="20">
-        <v>45.14462534538697</v>
-      </c>
-      <c r="E45" s="20">
-        <v>-0.46040799232020568</v>
-      </c>
-      <c r="F45" s="20">
-        <v>98.902634006845375</v>
-      </c>
-      <c r="G45" s="20">
-        <v>0.94456597482018534</v>
-      </c>
-      <c r="H45" s="20">
-        <v>0.13602890145700919</v>
-      </c>
-      <c r="I45" s="20">
-        <v>4.518796994871499E-2</v>
+      <c r="B45" s="21">
+        <v>32.998274021308887</v>
+      </c>
+      <c r="C45" s="21">
+        <v>3.5327653566194419</v>
+      </c>
+      <c r="D45" s="21">
+        <v>45.386641453166902</v>
+      </c>
+      <c r="E45" s="21">
+        <v>0.73547563417116057</v>
+      </c>
+      <c r="F45" s="21">
+        <v>98.318908766997453</v>
+      </c>
+      <c r="G45" s="21">
+        <v>1.3664989017566671</v>
+      </c>
+      <c r="H45" s="21">
+        <v>0.27003878238689832</v>
+      </c>
+      <c r="I45" s="21">
+        <v>0.11259164513982441</v>
       </c>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
@@ -10951,29 +10956,29 @@
       <c r="A46" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B46" s="20">
-        <v>31.13721906391498</v>
-      </c>
-      <c r="C46" s="20">
-        <v>-5.4485944694560047</v>
-      </c>
-      <c r="D46" s="20">
-        <v>49.750319386849426</v>
-      </c>
-      <c r="E46" s="20">
-        <v>-0.31159221662797099</v>
-      </c>
-      <c r="F46" s="20">
-        <v>98.920409235288872</v>
-      </c>
-      <c r="G46" s="20">
-        <v>0.98729994527226439</v>
-      </c>
-      <c r="H46" s="20">
-        <v>8.6569000912372837E-2</v>
-      </c>
-      <c r="I46" s="20">
-        <v>1.179979601269892E-2</v>
+      <c r="B46" s="21">
+        <v>31.096253709325371</v>
+      </c>
+      <c r="C46" s="21">
+        <v>2.418830387471107</v>
+      </c>
+      <c r="D46" s="21">
+        <v>52.979827829432963</v>
+      </c>
+      <c r="E46" s="21">
+        <v>-1.3799661021806801E-2</v>
+      </c>
+      <c r="F46" s="21">
+        <v>98.855523198885962</v>
+      </c>
+      <c r="G46" s="21">
+        <v>1.03861847799947</v>
+      </c>
+      <c r="H46" s="21">
+        <v>9.4481743498184348E-2</v>
+      </c>
+      <c r="I46" s="21">
+        <v>1.589646196979929E-2</v>
       </c>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
@@ -10984,28 +10989,28 @@
       <c r="A47" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B47" s="20">
-        <v>23.369988341752499</v>
-      </c>
-      <c r="C47" s="20">
-        <v>-3.5608</v>
-      </c>
-      <c r="D47" s="20">
-        <v>36.811100000000003</v>
-      </c>
-      <c r="E47" s="20">
-        <v>-4.6016000000000004</v>
-      </c>
-      <c r="F47" s="20">
-        <v>99.289297658861997</v>
-      </c>
-      <c r="G47" s="20">
-        <v>0.71070234113700004</v>
-      </c>
-      <c r="H47" s="20">
-        <v>0</v>
-      </c>
-      <c r="I47" s="20">
+      <c r="B47" s="21">
+        <v>24.398644741866601</v>
+      </c>
+      <c r="C47" s="21">
+        <v>9.5500000000000002E-2</v>
+      </c>
+      <c r="D47" s="21">
+        <v>39.016500000000001</v>
+      </c>
+      <c r="E47" s="21">
+        <v>-1.7730999999999999</v>
+      </c>
+      <c r="F47" s="21">
+        <v>99.032961046035993</v>
+      </c>
+      <c r="G47" s="21">
+        <v>0.95341868700599997</v>
+      </c>
+      <c r="H47" s="21">
+        <v>1.3620266957000001E-2</v>
+      </c>
+      <c r="I47" s="21">
         <v>0</v>
       </c>
       <c r="J47" s="4"/>
@@ -11017,28 +11022,28 @@
       <c r="A48" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B48" s="20">
-        <v>34.028674668803852</v>
-      </c>
-      <c r="C48" s="20">
-        <v>-10.10587922150131</v>
-      </c>
-      <c r="D48" s="20">
-        <v>56.801709202473113</v>
-      </c>
-      <c r="E48" s="20">
-        <v>-4.5220014824021098</v>
-      </c>
-      <c r="F48" s="20">
-        <v>99.814103694713964</v>
-      </c>
-      <c r="G48" s="20">
-        <v>0.18589630528509621</v>
-      </c>
-      <c r="H48" s="20">
-        <v>0</v>
-      </c>
-      <c r="I48" s="20">
+      <c r="B48" s="21">
+        <v>33.420778277803713</v>
+      </c>
+      <c r="C48" s="21">
+        <v>-0.84428104102771639</v>
+      </c>
+      <c r="D48" s="21">
+        <v>54.025509554150553</v>
+      </c>
+      <c r="E48" s="21">
+        <v>0.39375808876175739</v>
+      </c>
+      <c r="F48" s="21">
+        <v>99.777544944186815</v>
+      </c>
+      <c r="G48" s="21">
+        <v>0.18433379597501731</v>
+      </c>
+      <c r="H48" s="21">
+        <v>3.8121259837232822E-2</v>
+      </c>
+      <c r="I48" s="21">
         <v>0</v>
       </c>
       <c r="J48" s="4"/>
@@ -11050,28 +11055,28 @@
       <c r="A49" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B49" s="20">
-        <v>24.111482119563629</v>
-      </c>
-      <c r="C49" s="20">
-        <v>-7.1936525642706286</v>
-      </c>
-      <c r="D49" s="20">
-        <v>44.415942815840957</v>
-      </c>
-      <c r="E49" s="20">
-        <v>-3.389075425076316</v>
-      </c>
-      <c r="F49" s="20">
-        <v>99.573294111073693</v>
-      </c>
-      <c r="G49" s="20">
-        <v>0.42211228372749998</v>
-      </c>
-      <c r="H49" s="20">
-        <v>4.5936051981044839E-3</v>
-      </c>
-      <c r="I49" s="20">
+      <c r="B49" s="21">
+        <v>23.962424638410639</v>
+      </c>
+      <c r="C49" s="21">
+        <v>0.38168619007107452</v>
+      </c>
+      <c r="D49" s="21">
+        <v>47.629952486752487</v>
+      </c>
+      <c r="E49" s="21">
+        <v>0.33930083473825662</v>
+      </c>
+      <c r="F49" s="21">
+        <v>99.495491416446555</v>
+      </c>
+      <c r="G49" s="21">
+        <v>0.48797256051790161</v>
+      </c>
+      <c r="H49" s="21">
+        <v>1.653602303417125E-2</v>
+      </c>
+      <c r="I49" s="21">
         <v>0</v>
       </c>
       <c r="J49" s="4"/>
@@ -11083,29 +11088,29 @@
       <c r="A50" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B50" s="20">
-        <v>25.1656795271258</v>
-      </c>
-      <c r="C50" s="20">
-        <v>-6.8068278475058044</v>
-      </c>
-      <c r="D50" s="20">
-        <v>55.397747106706518</v>
-      </c>
-      <c r="E50" s="20">
-        <v>-4.969698003400663</v>
-      </c>
-      <c r="F50" s="20">
-        <v>98.735513631041982</v>
-      </c>
-      <c r="G50" s="20">
-        <v>1.001508800110017</v>
-      </c>
-      <c r="H50" s="20">
-        <v>0.26297756884710899</v>
-      </c>
-      <c r="I50" s="20">
-        <v>0</v>
+      <c r="B50" s="21">
+        <v>23.885385422716791</v>
+      </c>
+      <c r="C50" s="21">
+        <v>1.4183965657069139E-4</v>
+      </c>
+      <c r="D50" s="21">
+        <v>59.479569590384372</v>
+      </c>
+      <c r="E50" s="21">
+        <v>0.61050911479938019</v>
+      </c>
+      <c r="F50" s="21">
+        <v>97.960441914140063</v>
+      </c>
+      <c r="G50" s="21">
+        <v>1.496803556525943</v>
+      </c>
+      <c r="H50" s="21">
+        <v>0.5385929837242831</v>
+      </c>
+      <c r="I50" s="21">
+        <v>1.328039932554336E-2</v>
       </c>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
@@ -11116,29 +11121,29 @@
       <c r="A51" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B51" s="20">
-        <v>32.741645368305051</v>
-      </c>
-      <c r="C51" s="20">
-        <v>-8.3112779457748971</v>
-      </c>
-      <c r="D51" s="20">
-        <v>38.672589401635094</v>
-      </c>
-      <c r="E51" s="20">
-        <v>-2.0283991508866981</v>
-      </c>
-      <c r="F51" s="20">
-        <v>98.352766293939595</v>
-      </c>
-      <c r="G51" s="20">
-        <v>1.53982654489577</v>
-      </c>
-      <c r="H51" s="20">
-        <v>0.1074071611641176</v>
-      </c>
-      <c r="I51" s="20">
-        <v>0</v>
+      <c r="B51" s="21">
+        <v>33.514670687587802</v>
+      </c>
+      <c r="C51" s="21">
+        <v>2.0201020009244481</v>
+      </c>
+      <c r="D51" s="21">
+        <v>38.317595478031841</v>
+      </c>
+      <c r="E51" s="21">
+        <v>0.62521829218744607</v>
+      </c>
+      <c r="F51" s="21">
+        <v>98.121621727458361</v>
+      </c>
+      <c r="G51" s="21">
+        <v>1.665076092264699</v>
+      </c>
+      <c r="H51" s="21">
+        <v>0.17064174422115169</v>
+      </c>
+      <c r="I51" s="21">
+        <v>4.2660436055287923E-2</v>
       </c>
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
@@ -11149,29 +11154,29 @@
       <c r="A52" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B52" s="20">
-        <v>25.152893713609021</v>
-      </c>
-      <c r="C52" s="20">
-        <v>-4.2806564987104352</v>
-      </c>
-      <c r="D52" s="20">
-        <v>51.08676700141902</v>
-      </c>
-      <c r="E52" s="20">
-        <v>2.1572577260017769</v>
-      </c>
-      <c r="F52" s="20">
-        <v>98.962919057927692</v>
-      </c>
-      <c r="G52" s="20">
-        <v>1.0013195302767079</v>
-      </c>
-      <c r="H52" s="20">
-        <v>2.8609129436477379E-2</v>
-      </c>
-      <c r="I52" s="20">
-        <v>7.1522823591193439E-3</v>
+      <c r="B52" s="21">
+        <v>30.27595154980045</v>
+      </c>
+      <c r="C52" s="21">
+        <v>2.5784931188513882</v>
+      </c>
+      <c r="D52" s="21">
+        <v>56.615996846926663</v>
+      </c>
+      <c r="E52" s="21">
+        <v>3.1289158192793942</v>
+      </c>
+      <c r="F52" s="21">
+        <v>98.661276293653401</v>
+      </c>
+      <c r="G52" s="21">
+        <v>1.246642181571441</v>
+      </c>
+      <c r="H52" s="21">
+        <v>8.4998330561689192E-2</v>
+      </c>
+      <c r="I52" s="21">
+        <v>7.0831942134740979E-3</v>
       </c>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
@@ -11182,29 +11187,29 @@
       <c r="A53" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B53" s="20">
-        <v>25.38791053193734</v>
-      </c>
-      <c r="C53" s="20">
-        <v>-0.71668484649861641</v>
-      </c>
-      <c r="D53" s="20">
-        <v>42.58994215390566</v>
-      </c>
-      <c r="E53" s="20">
-        <v>1.5205639960893971</v>
-      </c>
-      <c r="F53" s="20">
-        <v>98.04719283970708</v>
-      </c>
-      <c r="G53" s="20">
-        <v>1.790073230268511</v>
-      </c>
-      <c r="H53" s="20">
-        <v>8.1366965012205042E-2</v>
-      </c>
-      <c r="I53" s="20">
-        <v>8.1366965012205042E-2</v>
+      <c r="B53" s="21">
+        <v>26.01792308327509</v>
+      </c>
+      <c r="C53" s="21">
+        <v>5.0138909760834238</v>
+      </c>
+      <c r="D53" s="21">
+        <v>45.961616181774517</v>
+      </c>
+      <c r="E53" s="21">
+        <v>2.3408503141428172</v>
+      </c>
+      <c r="F53" s="21">
+        <v>97.321428571428569</v>
+      </c>
+      <c r="G53" s="21">
+        <v>2.2727272727272729</v>
+      </c>
+      <c r="H53" s="21">
+        <v>0.32467532467532467</v>
+      </c>
+      <c r="I53" s="21">
+        <v>8.1168831168831168E-2</v>
       </c>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
@@ -11220,9 +11225,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC61B108-7690-FA48-BD1F-70BA8E6E6932}">
   <dimension ref="A51:A100"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -11284,21 +11287,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4E922D9-587A-2248-9CA1-A6E55F67A864}">
-  <dimension ref="A2:D59"/>
+  <dimension ref="A2:D63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="2" spans="1:4" ht="20" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" s="12" t="s">
@@ -11744,6 +11747,38 @@
       </c>
       <c r="C59" s="10">
         <v>0.33100000000000002</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B60" s="15">
+        <v>44303</v>
+      </c>
+      <c r="C60" s="16">
+        <v>0.32700000000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B61" s="15">
+        <v>44310</v>
+      </c>
+      <c r="C61" s="16">
+        <v>0.34699999999999998</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B62" s="15">
+        <v>44317</v>
+      </c>
+      <c r="C62" s="16">
+        <v>0.32700000000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B63" s="15">
+        <v>44323</v>
+      </c>
+      <c r="C63" s="16">
+        <v>0.33900000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>